<commit_message>
add functions and endpoint to generate list of athletes; fix protection on xlsx file;
</commit_message>
<xml_diff>
--- a/assets/Заявка.xlsx
+++ b/assets/Заявка.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Игорь\WebstormProjects\synchroreg\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3583B8-1285-4267-8139-639AE007D9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A35927-DCAC-435B-AF4D-21C903DF9F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заявка" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="Sportsmen" localSheetId="0">Заявка!$B$11:$B$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1182,89 +1181,101 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1275,8 +1286,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1289,98 +1301,83 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1402,37 +1399,39 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1775,7 +1774,7 @@
   <dimension ref="A1:V66"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1836,73 +1835,73 @@
       <c r="B7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="98"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
     </row>
     <row r="8" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="115" t="s">
+      <c r="D9" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="117" t="s">
+      <c r="E9" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="102" t="s">
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="106" t="s">
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="P9" s="107"/>
-      <c r="Q9" s="107"/>
-      <c r="R9" s="108"/>
-      <c r="S9" s="99" t="s">
+      <c r="P9" s="77"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="78"/>
+      <c r="S9" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="T9" s="96"/>
-      <c r="U9" s="68" t="s">
+      <c r="T9" s="65"/>
+      <c r="U9" s="134" t="s">
         <v>34</v>
       </c>
-      <c r="V9" s="96" t="s">
+      <c r="V9" s="65" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="35" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="110"/>
-      <c r="B10" s="112"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="116"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="90"/>
       <c r="E10" s="46" t="s">
         <v>10</v>
       </c>
@@ -1945,17 +1944,17 @@
       <c r="R10" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="100"/>
-      <c r="T10" s="101"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="97"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="135"/>
+      <c r="V10" s="66"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <v>1</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="122"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="27"/>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
@@ -1971,8 +1970,8 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="55"/>
-      <c r="S11" s="70"/>
-      <c r="T11" s="71"/>
+      <c r="S11" s="128"/>
+      <c r="T11" s="129"/>
       <c r="U11" s="61"/>
       <c r="V11" s="58"/>
     </row>
@@ -1997,8 +1996,8 @@
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="56"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="65"/>
+      <c r="S12" s="130"/>
+      <c r="T12" s="131"/>
       <c r="U12" s="62"/>
       <c r="V12" s="59"/>
     </row>
@@ -2023,8 +2022,8 @@
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="56"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="65"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="131"/>
       <c r="U13" s="62"/>
       <c r="V13" s="59"/>
     </row>
@@ -2049,8 +2048,8 @@
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="56"/>
-      <c r="S14" s="64"/>
-      <c r="T14" s="65"/>
+      <c r="S14" s="130"/>
+      <c r="T14" s="131"/>
       <c r="U14" s="62"/>
       <c r="V14" s="59"/>
     </row>
@@ -2075,8 +2074,8 @@
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="56"/>
-      <c r="S15" s="64"/>
-      <c r="T15" s="65"/>
+      <c r="S15" s="130"/>
+      <c r="T15" s="131"/>
       <c r="U15" s="62"/>
       <c r="V15" s="59"/>
     </row>
@@ -2101,8 +2100,8 @@
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="56"/>
-      <c r="S16" s="64"/>
-      <c r="T16" s="65"/>
+      <c r="S16" s="130"/>
+      <c r="T16" s="131"/>
       <c r="U16" s="62"/>
       <c r="V16" s="59"/>
     </row>
@@ -2127,8 +2126,8 @@
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="56"/>
-      <c r="S17" s="64"/>
-      <c r="T17" s="65"/>
+      <c r="S17" s="130"/>
+      <c r="T17" s="131"/>
       <c r="U17" s="62"/>
       <c r="V17" s="59"/>
     </row>
@@ -2153,8 +2152,8 @@
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="56"/>
-      <c r="S18" s="64"/>
-      <c r="T18" s="65"/>
+      <c r="S18" s="130"/>
+      <c r="T18" s="131"/>
       <c r="U18" s="62"/>
       <c r="V18" s="59"/>
     </row>
@@ -2179,8 +2178,8 @@
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="56"/>
-      <c r="S19" s="64"/>
-      <c r="T19" s="65"/>
+      <c r="S19" s="130"/>
+      <c r="T19" s="131"/>
       <c r="U19" s="62"/>
       <c r="V19" s="59"/>
     </row>
@@ -2205,8 +2204,8 @@
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="56"/>
-      <c r="S20" s="64"/>
-      <c r="T20" s="65"/>
+      <c r="S20" s="130"/>
+      <c r="T20" s="131"/>
       <c r="U20" s="62"/>
       <c r="V20" s="59"/>
     </row>
@@ -2231,8 +2230,8 @@
       <c r="P21" s="18"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="56"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="65"/>
+      <c r="S21" s="130"/>
+      <c r="T21" s="131"/>
       <c r="U21" s="62"/>
       <c r="V21" s="59"/>
     </row>
@@ -2257,8 +2256,8 @@
       <c r="P22" s="18"/>
       <c r="Q22" s="18"/>
       <c r="R22" s="56"/>
-      <c r="S22" s="64"/>
-      <c r="T22" s="65"/>
+      <c r="S22" s="130"/>
+      <c r="T22" s="131"/>
       <c r="U22" s="62"/>
       <c r="V22" s="59"/>
     </row>
@@ -2283,8 +2282,8 @@
       <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="56"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="65"/>
+      <c r="S23" s="130"/>
+      <c r="T23" s="131"/>
       <c r="U23" s="62"/>
       <c r="V23" s="59"/>
     </row>
@@ -2309,8 +2308,8 @@
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
       <c r="R24" s="56"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="65"/>
+      <c r="S24" s="130"/>
+      <c r="T24" s="131"/>
       <c r="U24" s="62"/>
       <c r="V24" s="59"/>
     </row>
@@ -2335,8 +2334,8 @@
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="56"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="65"/>
+      <c r="S25" s="130"/>
+      <c r="T25" s="131"/>
       <c r="U25" s="62"/>
       <c r="V25" s="59"/>
     </row>
@@ -2361,8 +2360,8 @@
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="56"/>
-      <c r="S26" s="64"/>
-      <c r="T26" s="65"/>
+      <c r="S26" s="130"/>
+      <c r="T26" s="131"/>
       <c r="U26" s="62"/>
       <c r="V26" s="59"/>
     </row>
@@ -2387,8 +2386,8 @@
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="56"/>
-      <c r="S27" s="64"/>
-      <c r="T27" s="65"/>
+      <c r="S27" s="130"/>
+      <c r="T27" s="131"/>
       <c r="U27" s="62"/>
       <c r="V27" s="59"/>
     </row>
@@ -2413,8 +2412,8 @@
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="56"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="65"/>
+      <c r="S28" s="130"/>
+      <c r="T28" s="131"/>
       <c r="U28" s="62"/>
       <c r="V28" s="59"/>
     </row>
@@ -2439,8 +2438,8 @@
       <c r="P29" s="18"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="56"/>
-      <c r="S29" s="64"/>
-      <c r="T29" s="65"/>
+      <c r="S29" s="130"/>
+      <c r="T29" s="131"/>
       <c r="U29" s="62"/>
       <c r="V29" s="59"/>
     </row>
@@ -2465,8 +2464,8 @@
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="56"/>
-      <c r="S30" s="64"/>
-      <c r="T30" s="65"/>
+      <c r="S30" s="130"/>
+      <c r="T30" s="131"/>
       <c r="U30" s="62"/>
       <c r="V30" s="59"/>
     </row>
@@ -2491,8 +2490,8 @@
       <c r="P31" s="18"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="56"/>
-      <c r="S31" s="64"/>
-      <c r="T31" s="65"/>
+      <c r="S31" s="130"/>
+      <c r="T31" s="131"/>
       <c r="U31" s="62"/>
       <c r="V31" s="59"/>
     </row>
@@ -2517,8 +2516,8 @@
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="56"/>
-      <c r="S32" s="64"/>
-      <c r="T32" s="65"/>
+      <c r="S32" s="130"/>
+      <c r="T32" s="131"/>
       <c r="U32" s="62"/>
       <c r="V32" s="59"/>
     </row>
@@ -2543,8 +2542,8 @@
       <c r="P33" s="18"/>
       <c r="Q33" s="18"/>
       <c r="R33" s="56"/>
-      <c r="S33" s="64"/>
-      <c r="T33" s="65"/>
+      <c r="S33" s="130"/>
+      <c r="T33" s="131"/>
       <c r="U33" s="62"/>
       <c r="V33" s="59"/>
     </row>
@@ -2569,8 +2568,8 @@
       <c r="P34" s="18"/>
       <c r="Q34" s="18"/>
       <c r="R34" s="56"/>
-      <c r="S34" s="64"/>
-      <c r="T34" s="65"/>
+      <c r="S34" s="130"/>
+      <c r="T34" s="131"/>
       <c r="U34" s="62"/>
       <c r="V34" s="59"/>
     </row>
@@ -2595,8 +2594,8 @@
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="56"/>
-      <c r="S35" s="64"/>
-      <c r="T35" s="65"/>
+      <c r="S35" s="130"/>
+      <c r="T35" s="131"/>
       <c r="U35" s="62"/>
       <c r="V35" s="59"/>
     </row>
@@ -2621,8 +2620,8 @@
       <c r="P36" s="18"/>
       <c r="Q36" s="18"/>
       <c r="R36" s="56"/>
-      <c r="S36" s="64"/>
-      <c r="T36" s="65"/>
+      <c r="S36" s="130"/>
+      <c r="T36" s="131"/>
       <c r="U36" s="62"/>
       <c r="V36" s="59"/>
     </row>
@@ -2647,8 +2646,8 @@
       <c r="P37" s="18"/>
       <c r="Q37" s="18"/>
       <c r="R37" s="56"/>
-      <c r="S37" s="64"/>
-      <c r="T37" s="65"/>
+      <c r="S37" s="130"/>
+      <c r="T37" s="131"/>
       <c r="U37" s="62"/>
       <c r="V37" s="59"/>
     </row>
@@ -2673,8 +2672,8 @@
       <c r="P38" s="18"/>
       <c r="Q38" s="18"/>
       <c r="R38" s="56"/>
-      <c r="S38" s="64"/>
-      <c r="T38" s="65"/>
+      <c r="S38" s="130"/>
+      <c r="T38" s="131"/>
       <c r="U38" s="62"/>
       <c r="V38" s="59"/>
     </row>
@@ -2699,8 +2698,8 @@
       <c r="P39" s="18"/>
       <c r="Q39" s="18"/>
       <c r="R39" s="56"/>
-      <c r="S39" s="64"/>
-      <c r="T39" s="65"/>
+      <c r="S39" s="130"/>
+      <c r="T39" s="131"/>
       <c r="U39" s="62"/>
       <c r="V39" s="59"/>
     </row>
@@ -2725,8 +2724,8 @@
       <c r="P40" s="18"/>
       <c r="Q40" s="18"/>
       <c r="R40" s="56"/>
-      <c r="S40" s="64"/>
-      <c r="T40" s="65"/>
+      <c r="S40" s="130"/>
+      <c r="T40" s="131"/>
       <c r="U40" s="62"/>
       <c r="V40" s="59"/>
     </row>
@@ -2751,8 +2750,8 @@
       <c r="P41" s="18"/>
       <c r="Q41" s="18"/>
       <c r="R41" s="56"/>
-      <c r="S41" s="64"/>
-      <c r="T41" s="65"/>
+      <c r="S41" s="130"/>
+      <c r="T41" s="131"/>
       <c r="U41" s="62"/>
       <c r="V41" s="59"/>
     </row>
@@ -2777,8 +2776,8 @@
       <c r="P42" s="18"/>
       <c r="Q42" s="18"/>
       <c r="R42" s="56"/>
-      <c r="S42" s="64"/>
-      <c r="T42" s="65"/>
+      <c r="S42" s="130"/>
+      <c r="T42" s="131"/>
       <c r="U42" s="62"/>
       <c r="V42" s="59"/>
     </row>
@@ -2803,8 +2802,8 @@
       <c r="P43" s="18"/>
       <c r="Q43" s="18"/>
       <c r="R43" s="56"/>
-      <c r="S43" s="64"/>
-      <c r="T43" s="65"/>
+      <c r="S43" s="130"/>
+      <c r="T43" s="131"/>
       <c r="U43" s="62"/>
       <c r="V43" s="59"/>
     </row>
@@ -2829,8 +2828,8 @@
       <c r="P44" s="18"/>
       <c r="Q44" s="18"/>
       <c r="R44" s="56"/>
-      <c r="S44" s="64"/>
-      <c r="T44" s="65"/>
+      <c r="S44" s="130"/>
+      <c r="T44" s="131"/>
       <c r="U44" s="62"/>
       <c r="V44" s="59"/>
     </row>
@@ -2855,8 +2854,8 @@
       <c r="P45" s="18"/>
       <c r="Q45" s="18"/>
       <c r="R45" s="56"/>
-      <c r="S45" s="64"/>
-      <c r="T45" s="65"/>
+      <c r="S45" s="130"/>
+      <c r="T45" s="131"/>
       <c r="U45" s="62"/>
       <c r="V45" s="59"/>
     </row>
@@ -2881,8 +2880,8 @@
       <c r="P46" s="18"/>
       <c r="Q46" s="18"/>
       <c r="R46" s="56"/>
-      <c r="S46" s="64"/>
-      <c r="T46" s="65"/>
+      <c r="S46" s="130"/>
+      <c r="T46" s="131"/>
       <c r="U46" s="62"/>
       <c r="V46" s="59"/>
     </row>
@@ -2907,8 +2906,8 @@
       <c r="P47" s="18"/>
       <c r="Q47" s="18"/>
       <c r="R47" s="56"/>
-      <c r="S47" s="64"/>
-      <c r="T47" s="65"/>
+      <c r="S47" s="130"/>
+      <c r="T47" s="131"/>
       <c r="U47" s="62"/>
       <c r="V47" s="59"/>
     </row>
@@ -2933,8 +2932,8 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="57"/>
-      <c r="S48" s="66"/>
-      <c r="T48" s="67"/>
+      <c r="S48" s="132"/>
+      <c r="T48" s="133"/>
       <c r="U48" s="63"/>
       <c r="V48" s="60"/>
     </row>
@@ -2944,249 +2943,249 @@
     </row>
     <row r="50" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="45"/>
-      <c r="B50" s="87" t="s">
+      <c r="B50" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="88"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="90" t="s">
+      <c r="C50" s="95"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="91"/>
-      <c r="G50" s="91"/>
-      <c r="H50" s="90" t="s">
+      <c r="F50" s="98"/>
+      <c r="G50" s="98"/>
+      <c r="H50" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="I50" s="105"/>
-      <c r="J50" s="91" t="s">
+      <c r="I50" s="75"/>
+      <c r="J50" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="K50" s="91"/>
-      <c r="L50" s="90" t="s">
+      <c r="K50" s="98"/>
+      <c r="L50" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="M50" s="91"/>
-      <c r="N50" s="91"/>
-      <c r="O50" s="91"/>
-      <c r="P50" s="75" t="s">
+      <c r="M50" s="98"/>
+      <c r="N50" s="98"/>
+      <c r="O50" s="98"/>
+      <c r="P50" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="Q50" s="76"/>
-      <c r="R50" s="76"/>
-      <c r="S50" s="77"/>
-      <c r="T50" s="72" t="s">
+      <c r="Q50" s="120"/>
+      <c r="R50" s="120"/>
+      <c r="S50" s="121"/>
+      <c r="T50" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="U50" s="73"/>
-      <c r="V50" s="74"/>
+      <c r="U50" s="117"/>
+      <c r="V50" s="118"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="42">
         <v>1</v>
       </c>
-      <c r="B51" s="82"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="92"/>
-      <c r="F51" s="93"/>
-      <c r="G51" s="93"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="83"/>
-      <c r="J51" s="85"/>
-      <c r="K51" s="83"/>
-      <c r="L51" s="82"/>
-      <c r="M51" s="85"/>
-      <c r="N51" s="85"/>
-      <c r="O51" s="85"/>
-      <c r="P51" s="123"/>
-      <c r="Q51" s="124"/>
-      <c r="R51" s="124"/>
-      <c r="S51" s="125"/>
-      <c r="T51" s="126"/>
-      <c r="U51" s="127"/>
-      <c r="V51" s="125"/>
+      <c r="B51" s="101"/>
+      <c r="C51" s="102"/>
+      <c r="D51" s="106"/>
+      <c r="E51" s="99"/>
+      <c r="F51" s="100"/>
+      <c r="G51" s="100"/>
+      <c r="H51" s="101"/>
+      <c r="I51" s="106"/>
+      <c r="J51" s="102"/>
+      <c r="K51" s="106"/>
+      <c r="L51" s="101"/>
+      <c r="M51" s="102"/>
+      <c r="N51" s="102"/>
+      <c r="O51" s="102"/>
+      <c r="P51" s="122"/>
+      <c r="Q51" s="123"/>
+      <c r="R51" s="123"/>
+      <c r="S51" s="124"/>
+      <c r="T51" s="125"/>
+      <c r="U51" s="126"/>
+      <c r="V51" s="124"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="43">
         <v>2</v>
       </c>
-      <c r="B52" s="84"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="79"/>
-      <c r="E52" s="94"/>
-      <c r="F52" s="95"/>
-      <c r="G52" s="95"/>
-      <c r="H52" s="84"/>
-      <c r="I52" s="79"/>
-      <c r="J52" s="78"/>
-      <c r="K52" s="79"/>
-      <c r="L52" s="84"/>
-      <c r="M52" s="78"/>
-      <c r="N52" s="78"/>
-      <c r="O52" s="78"/>
-      <c r="P52" s="128"/>
-      <c r="Q52" s="129"/>
-      <c r="R52" s="129"/>
-      <c r="S52" s="130"/>
-      <c r="T52" s="131"/>
-      <c r="U52" s="78"/>
-      <c r="V52" s="130"/>
+      <c r="B52" s="79"/>
+      <c r="C52" s="97"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="80"/>
+      <c r="J52" s="97"/>
+      <c r="K52" s="80"/>
+      <c r="L52" s="79"/>
+      <c r="M52" s="97"/>
+      <c r="N52" s="97"/>
+      <c r="O52" s="97"/>
+      <c r="P52" s="111"/>
+      <c r="Q52" s="112"/>
+      <c r="R52" s="112"/>
+      <c r="S52" s="113"/>
+      <c r="T52" s="127"/>
+      <c r="U52" s="97"/>
+      <c r="V52" s="113"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="43">
         <v>3</v>
       </c>
-      <c r="B53" s="84"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="95"/>
-      <c r="G53" s="95"/>
-      <c r="H53" s="84"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="78"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="84"/>
-      <c r="M53" s="78"/>
-      <c r="N53" s="78"/>
-      <c r="O53" s="78"/>
-      <c r="P53" s="128"/>
-      <c r="Q53" s="129"/>
-      <c r="R53" s="129"/>
-      <c r="S53" s="130"/>
-      <c r="T53" s="131"/>
-      <c r="U53" s="78"/>
-      <c r="V53" s="130"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="82"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="80"/>
+      <c r="J53" s="97"/>
+      <c r="K53" s="80"/>
+      <c r="L53" s="79"/>
+      <c r="M53" s="97"/>
+      <c r="N53" s="97"/>
+      <c r="O53" s="97"/>
+      <c r="P53" s="111"/>
+      <c r="Q53" s="112"/>
+      <c r="R53" s="112"/>
+      <c r="S53" s="113"/>
+      <c r="T53" s="127"/>
+      <c r="U53" s="97"/>
+      <c r="V53" s="113"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="43">
         <v>4</v>
       </c>
-      <c r="B54" s="84"/>
-      <c r="C54" s="78"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="94"/>
-      <c r="F54" s="95"/>
-      <c r="G54" s="95"/>
-      <c r="H54" s="84"/>
-      <c r="I54" s="79"/>
-      <c r="J54" s="78"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="84"/>
-      <c r="M54" s="78"/>
-      <c r="N54" s="78"/>
-      <c r="O54" s="78"/>
-      <c r="P54" s="128"/>
-      <c r="Q54" s="129"/>
-      <c r="R54" s="129"/>
-      <c r="S54" s="130"/>
-      <c r="T54" s="131"/>
-      <c r="U54" s="78"/>
-      <c r="V54" s="130"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="97"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="82"/>
+      <c r="G54" s="82"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="80"/>
+      <c r="J54" s="97"/>
+      <c r="K54" s="80"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="97"/>
+      <c r="N54" s="97"/>
+      <c r="O54" s="97"/>
+      <c r="P54" s="111"/>
+      <c r="Q54" s="112"/>
+      <c r="R54" s="112"/>
+      <c r="S54" s="113"/>
+      <c r="T54" s="127"/>
+      <c r="U54" s="97"/>
+      <c r="V54" s="113"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="43">
         <v>5</v>
       </c>
-      <c r="B55" s="84"/>
-      <c r="C55" s="78"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="94"/>
-      <c r="F55" s="95"/>
-      <c r="G55" s="95"/>
-      <c r="H55" s="84"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="78"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="84"/>
-      <c r="M55" s="78"/>
-      <c r="N55" s="78"/>
-      <c r="O55" s="78"/>
-      <c r="P55" s="128"/>
-      <c r="Q55" s="129"/>
-      <c r="R55" s="129"/>
-      <c r="S55" s="130"/>
-      <c r="T55" s="131"/>
-      <c r="U55" s="78"/>
-      <c r="V55" s="130"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="97"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="82"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="80"/>
+      <c r="J55" s="97"/>
+      <c r="K55" s="80"/>
+      <c r="L55" s="79"/>
+      <c r="M55" s="97"/>
+      <c r="N55" s="97"/>
+      <c r="O55" s="97"/>
+      <c r="P55" s="111"/>
+      <c r="Q55" s="112"/>
+      <c r="R55" s="112"/>
+      <c r="S55" s="113"/>
+      <c r="T55" s="127"/>
+      <c r="U55" s="97"/>
+      <c r="V55" s="113"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="43">
         <v>6</v>
       </c>
-      <c r="B56" s="84"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="94"/>
-      <c r="F56" s="95"/>
-      <c r="G56" s="95"/>
-      <c r="H56" s="84"/>
-      <c r="I56" s="79"/>
-      <c r="J56" s="78"/>
-      <c r="K56" s="79"/>
-      <c r="L56" s="84"/>
-      <c r="M56" s="78"/>
-      <c r="N56" s="78"/>
-      <c r="O56" s="78"/>
-      <c r="P56" s="128"/>
-      <c r="Q56" s="129"/>
-      <c r="R56" s="129"/>
-      <c r="S56" s="130"/>
-      <c r="T56" s="131"/>
-      <c r="U56" s="78"/>
-      <c r="V56" s="130"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="97"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="81"/>
+      <c r="F56" s="82"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="80"/>
+      <c r="J56" s="97"/>
+      <c r="K56" s="80"/>
+      <c r="L56" s="79"/>
+      <c r="M56" s="97"/>
+      <c r="N56" s="97"/>
+      <c r="O56" s="97"/>
+      <c r="P56" s="111"/>
+      <c r="Q56" s="112"/>
+      <c r="R56" s="112"/>
+      <c r="S56" s="113"/>
+      <c r="T56" s="127"/>
+      <c r="U56" s="97"/>
+      <c r="V56" s="113"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="43">
         <v>7</v>
       </c>
-      <c r="B57" s="84"/>
-      <c r="C57" s="78"/>
-      <c r="D57" s="79"/>
-      <c r="E57" s="94"/>
-      <c r="F57" s="95"/>
-      <c r="G57" s="95"/>
-      <c r="H57" s="84"/>
-      <c r="I57" s="79"/>
-      <c r="J57" s="78"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="84"/>
-      <c r="M57" s="78"/>
-      <c r="N57" s="78"/>
-      <c r="O57" s="78"/>
-      <c r="P57" s="128"/>
-      <c r="Q57" s="129"/>
-      <c r="R57" s="129"/>
-      <c r="S57" s="130"/>
-      <c r="T57" s="131"/>
-      <c r="U57" s="78"/>
-      <c r="V57" s="130"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="97"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="81"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="79"/>
+      <c r="I57" s="80"/>
+      <c r="J57" s="97"/>
+      <c r="K57" s="80"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="97"/>
+      <c r="N57" s="97"/>
+      <c r="O57" s="97"/>
+      <c r="P57" s="111"/>
+      <c r="Q57" s="112"/>
+      <c r="R57" s="112"/>
+      <c r="S57" s="113"/>
+      <c r="T57" s="127"/>
+      <c r="U57" s="97"/>
+      <c r="V57" s="113"/>
     </row>
     <row r="58" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="44">
         <v>8</v>
       </c>
-      <c r="B58" s="86"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="81"/>
-      <c r="E58" s="120"/>
-      <c r="F58" s="121"/>
-      <c r="G58" s="121"/>
-      <c r="H58" s="86"/>
-      <c r="I58" s="81"/>
-      <c r="J58" s="80"/>
-      <c r="K58" s="81"/>
-      <c r="L58" s="86"/>
-      <c r="M58" s="80"/>
-      <c r="N58" s="80"/>
-      <c r="O58" s="80"/>
-      <c r="P58" s="132"/>
-      <c r="Q58" s="133"/>
-      <c r="R58" s="133"/>
-      <c r="S58" s="134"/>
-      <c r="T58" s="135"/>
-      <c r="U58" s="80"/>
-      <c r="V58" s="134"/>
+      <c r="B58" s="103"/>
+      <c r="C58" s="104"/>
+      <c r="D58" s="105"/>
+      <c r="E58" s="107"/>
+      <c r="F58" s="108"/>
+      <c r="G58" s="108"/>
+      <c r="H58" s="103"/>
+      <c r="I58" s="105"/>
+      <c r="J58" s="104"/>
+      <c r="K58" s="105"/>
+      <c r="L58" s="103"/>
+      <c r="M58" s="104"/>
+      <c r="N58" s="104"/>
+      <c r="O58" s="104"/>
+      <c r="P58" s="114"/>
+      <c r="Q58" s="115"/>
+      <c r="R58" s="115"/>
+      <c r="S58" s="110"/>
+      <c r="T58" s="109"/>
+      <c r="U58" s="104"/>
+      <c r="V58" s="110"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="33"/>
@@ -3268,8 +3267,96 @@
       <c r="U66" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="lgcwSewUShOIgExfQZnmyE0f/ACkq+1dgP3cfYrXpc+E9waqRzTWmkkTEvaBm8pURYOqrqZqea2dedjFc0jupA==" saltValue="erX5pIgarUfqTfgUWZVy/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="112">
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="S45:T45"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S39:T39"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="T50:V50"/>
+    <mergeCell ref="P50:S50"/>
+    <mergeCell ref="P51:S51"/>
+    <mergeCell ref="P52:S52"/>
+    <mergeCell ref="P53:S53"/>
+    <mergeCell ref="T51:V51"/>
+    <mergeCell ref="T52:V52"/>
+    <mergeCell ref="T53:V53"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S46:T46"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="T58:V58"/>
+    <mergeCell ref="P54:S54"/>
+    <mergeCell ref="P55:S55"/>
+    <mergeCell ref="P56:S56"/>
+    <mergeCell ref="P57:S57"/>
+    <mergeCell ref="P58:S58"/>
+    <mergeCell ref="T54:V54"/>
+    <mergeCell ref="T55:V55"/>
+    <mergeCell ref="T56:V56"/>
+    <mergeCell ref="T57:V57"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="L55:O55"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="L56:O56"/>
+    <mergeCell ref="L57:O57"/>
+    <mergeCell ref="L58:O58"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
     <mergeCell ref="V9:V10"/>
     <mergeCell ref="C7:R7"/>
     <mergeCell ref="S9:T10"/>
@@ -3294,94 +3381,6 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="E53:G53"/>
     <mergeCell ref="E54:G54"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="L55:O55"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="L56:O56"/>
-    <mergeCell ref="L57:O57"/>
-    <mergeCell ref="L58:O58"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="T58:V58"/>
-    <mergeCell ref="P54:S54"/>
-    <mergeCell ref="P55:S55"/>
-    <mergeCell ref="P56:S56"/>
-    <mergeCell ref="P57:S57"/>
-    <mergeCell ref="P58:S58"/>
-    <mergeCell ref="T50:V50"/>
-    <mergeCell ref="P50:S50"/>
-    <mergeCell ref="P51:S51"/>
-    <mergeCell ref="P52:S52"/>
-    <mergeCell ref="P53:S53"/>
-    <mergeCell ref="T51:V51"/>
-    <mergeCell ref="T52:V52"/>
-    <mergeCell ref="T53:V53"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="T54:V54"/>
-    <mergeCell ref="T55:V55"/>
-    <mergeCell ref="T56:V56"/>
-    <mergeCell ref="T57:V57"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S46:T46"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S39:T39"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S30:T30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations xWindow="727" yWindow="303" count="13">

</xml_diff>

<commit_message>
Fixed compatibility with old program;
</commit_message>
<xml_diff>
--- a/assets/Заявка.xlsx
+++ b/assets/Заявка.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Игорь\WebstormProjects\synchroreg\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Игорь\WebstormProjects\synchroreg\assets\Заявки\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27C1C3D-92BA-41E3-A866-D5A9710EEFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735D4F75-E7EE-4078-95E6-4036EEBBA296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>ТЕХНИЧЕСКАЯ ЗАЯВКА</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Приказ о присвоении категории</t>
-  </si>
-  <si>
-    <t>Приказ о продлении категории</t>
   </si>
   <si>
     <t>ФИО спортсмена</t>
@@ -229,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -679,19 +676,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -938,15 +922,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -964,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1088,10 +1063,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1102,146 +1077,252 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1249,88 +1330,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1357,28 +1362,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1391,43 +1374,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1767,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:R7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1793,111 +1742,110 @@
     <col min="17" max="17" width="9.5703125" style="30" customWidth="1"/>
     <col min="18" max="18" width="8" style="30" customWidth="1"/>
     <col min="19" max="19" width="23.42578125" style="30" customWidth="1"/>
-    <col min="21" max="21" width="18.42578125" customWidth="1"/>
-    <col min="22" max="22" width="23.140625" style="30" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" style="32" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="32"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="23.140625" style="30" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="32" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="31" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="31"/>
     </row>
-    <row r="4" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="31"/>
     </row>
-    <row r="5" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="31"/>
     </row>
-    <row r="7" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="91"/>
-      <c r="P7" s="91"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="91"/>
-    </row>
-    <row r="8" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="64" t="s">
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
+      <c r="P7" s="89"/>
+      <c r="Q7" s="89"/>
+      <c r="R7" s="89"/>
+    </row>
+    <row r="8" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="D9" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="94"/>
+      <c r="O9" s="97" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="98"/>
+      <c r="Q9" s="98"/>
+      <c r="R9" s="99"/>
+      <c r="S9" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="72" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
-      <c r="N9" s="97"/>
-      <c r="O9" s="99" t="s">
-        <v>15</v>
-      </c>
-      <c r="P9" s="100"/>
-      <c r="Q9" s="100"/>
-      <c r="R9" s="101"/>
-      <c r="S9" s="92" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" s="89"/>
-      <c r="U9" s="133" t="s">
-        <v>34</v>
-      </c>
-      <c r="V9" s="89" t="s">
+      <c r="U9" s="87" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="34" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="71"/>
+    <row r="10" spans="1:21" s="34" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="71"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="77"/>
       <c r="E10" s="45" t="s">
         <v>10</v>
       </c>
@@ -1940,12 +1888,11 @@
       <c r="R10" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="93"/>
-      <c r="T10" s="94"/>
-      <c r="U10" s="134"/>
-      <c r="V10" s="90"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S10" s="91"/>
+      <c r="T10" s="106"/>
+      <c r="U10" s="88"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>1</v>
       </c>
@@ -1966,12 +1913,11 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="54"/>
-      <c r="S11" s="127"/>
-      <c r="T11" s="128"/>
-      <c r="U11" s="60"/>
-      <c r="V11" s="57"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S11" s="67"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="57"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>2</v>
       </c>
@@ -1987,17 +1933,16 @@
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
-      <c r="N12" s="9"/>
+      <c r="N12" s="16"/>
       <c r="O12" s="17"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="55"/>
-      <c r="S12" s="129"/>
-      <c r="T12" s="130"/>
-      <c r="U12" s="61"/>
-      <c r="V12" s="58"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S12" s="64"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="58"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>3</v>
       </c>
@@ -2013,17 +1958,16 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
-      <c r="N13" s="9"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="17"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="55"/>
-      <c r="S13" s="129"/>
-      <c r="T13" s="130"/>
-      <c r="U13" s="61"/>
-      <c r="V13" s="58"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S13" s="64"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="58"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>4</v>
       </c>
@@ -2039,17 +1983,16 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="9"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="17"/>
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="55"/>
-      <c r="S14" s="129"/>
-      <c r="T14" s="130"/>
-      <c r="U14" s="61"/>
-      <c r="V14" s="58"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S14" s="64"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="58"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>5</v>
       </c>
@@ -2065,17 +2008,16 @@
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="9"/>
+      <c r="N15" s="16"/>
       <c r="O15" s="17"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="55"/>
-      <c r="S15" s="129"/>
-      <c r="T15" s="130"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="58"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S15" s="64"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="58"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>6</v>
       </c>
@@ -2091,17 +2033,16 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="9"/>
+      <c r="N16" s="16"/>
       <c r="O16" s="17"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="55"/>
-      <c r="S16" s="129"/>
-      <c r="T16" s="130"/>
-      <c r="U16" s="61"/>
-      <c r="V16" s="58"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S16" s="64"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="58"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>7</v>
       </c>
@@ -2117,17 +2058,16 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="9"/>
+      <c r="N17" s="16"/>
       <c r="O17" s="17"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="55"/>
-      <c r="S17" s="129"/>
-      <c r="T17" s="130"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="58"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S17" s="64"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="58"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>8</v>
       </c>
@@ -2143,17 +2083,16 @@
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="9"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="17"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="55"/>
-      <c r="S18" s="129"/>
-      <c r="T18" s="130"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="58"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S18" s="64"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="58"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>9</v>
       </c>
@@ -2169,17 +2108,16 @@
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
-      <c r="N19" s="9"/>
+      <c r="N19" s="16"/>
       <c r="O19" s="17"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="55"/>
-      <c r="S19" s="129"/>
-      <c r="T19" s="130"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="58"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S19" s="64"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="58"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>10</v>
       </c>
@@ -2195,17 +2133,16 @@
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
-      <c r="N20" s="9"/>
+      <c r="N20" s="16"/>
       <c r="O20" s="17"/>
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="55"/>
-      <c r="S20" s="129"/>
-      <c r="T20" s="130"/>
-      <c r="U20" s="61"/>
-      <c r="V20" s="58"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S20" s="64"/>
+      <c r="T20" s="60"/>
+      <c r="U20" s="58"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>11</v>
       </c>
@@ -2221,17 +2158,16 @@
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
-      <c r="N21" s="9"/>
+      <c r="N21" s="16"/>
       <c r="O21" s="17"/>
       <c r="P21" s="18"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="55"/>
-      <c r="S21" s="129"/>
-      <c r="T21" s="130"/>
-      <c r="U21" s="61"/>
-      <c r="V21" s="58"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S21" s="64"/>
+      <c r="T21" s="60"/>
+      <c r="U21" s="58"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>12</v>
       </c>
@@ -2247,17 +2183,16 @@
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
-      <c r="N22" s="9"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="17"/>
       <c r="P22" s="18"/>
       <c r="Q22" s="18"/>
       <c r="R22" s="55"/>
-      <c r="S22" s="129"/>
-      <c r="T22" s="130"/>
-      <c r="U22" s="61"/>
-      <c r="V22" s="58"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S22" s="64"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="58"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>13</v>
       </c>
@@ -2278,12 +2213,11 @@
       <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="55"/>
-      <c r="S23" s="129"/>
-      <c r="T23" s="130"/>
-      <c r="U23" s="61"/>
-      <c r="V23" s="58"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S23" s="65"/>
+      <c r="T23" s="61"/>
+      <c r="U23" s="58"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>14</v>
       </c>
@@ -2304,12 +2238,11 @@
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
       <c r="R24" s="55"/>
-      <c r="S24" s="129"/>
-      <c r="T24" s="130"/>
-      <c r="U24" s="61"/>
-      <c r="V24" s="58"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S24" s="65"/>
+      <c r="T24" s="61"/>
+      <c r="U24" s="58"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>15</v>
       </c>
@@ -2330,12 +2263,11 @@
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="55"/>
-      <c r="S25" s="129"/>
-      <c r="T25" s="130"/>
-      <c r="U25" s="61"/>
-      <c r="V25" s="58"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S25" s="65"/>
+      <c r="T25" s="61"/>
+      <c r="U25" s="58"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>16</v>
       </c>
@@ -2356,12 +2288,11 @@
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="55"/>
-      <c r="S26" s="129"/>
-      <c r="T26" s="130"/>
-      <c r="U26" s="61"/>
-      <c r="V26" s="58"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S26" s="65"/>
+      <c r="T26" s="61"/>
+      <c r="U26" s="58"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>17</v>
       </c>
@@ -2382,12 +2313,11 @@
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="55"/>
-      <c r="S27" s="129"/>
-      <c r="T27" s="130"/>
-      <c r="U27" s="61"/>
-      <c r="V27" s="58"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S27" s="65"/>
+      <c r="T27" s="61"/>
+      <c r="U27" s="58"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
         <v>18</v>
       </c>
@@ -2408,12 +2338,11 @@
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="55"/>
-      <c r="S28" s="129"/>
-      <c r="T28" s="130"/>
-      <c r="U28" s="61"/>
-      <c r="V28" s="58"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S28" s="65"/>
+      <c r="T28" s="61"/>
+      <c r="U28" s="58"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>19</v>
       </c>
@@ -2434,12 +2363,11 @@
       <c r="P29" s="18"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="55"/>
-      <c r="S29" s="129"/>
-      <c r="T29" s="130"/>
-      <c r="U29" s="61"/>
-      <c r="V29" s="58"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S29" s="65"/>
+      <c r="T29" s="61"/>
+      <c r="U29" s="58"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
         <v>20</v>
       </c>
@@ -2460,12 +2388,11 @@
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="55"/>
-      <c r="S30" s="129"/>
-      <c r="T30" s="130"/>
-      <c r="U30" s="61"/>
-      <c r="V30" s="58"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S30" s="65"/>
+      <c r="T30" s="61"/>
+      <c r="U30" s="58"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
         <v>21</v>
       </c>
@@ -2486,12 +2413,11 @@
       <c r="P31" s="18"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="55"/>
-      <c r="S31" s="129"/>
-      <c r="T31" s="130"/>
-      <c r="U31" s="61"/>
-      <c r="V31" s="58"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S31" s="65"/>
+      <c r="T31" s="61"/>
+      <c r="U31" s="58"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="35">
         <v>22</v>
       </c>
@@ -2512,12 +2438,11 @@
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="55"/>
-      <c r="S32" s="129"/>
-      <c r="T32" s="130"/>
-      <c r="U32" s="61"/>
-      <c r="V32" s="58"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S32" s="65"/>
+      <c r="T32" s="61"/>
+      <c r="U32" s="58"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="35">
         <v>23</v>
       </c>
@@ -2538,12 +2463,11 @@
       <c r="P33" s="18"/>
       <c r="Q33" s="18"/>
       <c r="R33" s="55"/>
-      <c r="S33" s="129"/>
-      <c r="T33" s="130"/>
-      <c r="U33" s="61"/>
-      <c r="V33" s="58"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S33" s="65"/>
+      <c r="T33" s="61"/>
+      <c r="U33" s="58"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="35">
         <v>24</v>
       </c>
@@ -2564,12 +2488,11 @@
       <c r="P34" s="18"/>
       <c r="Q34" s="18"/>
       <c r="R34" s="55"/>
-      <c r="S34" s="129"/>
-      <c r="T34" s="130"/>
-      <c r="U34" s="61"/>
-      <c r="V34" s="58"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S34" s="65"/>
+      <c r="T34" s="61"/>
+      <c r="U34" s="58"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="35">
         <v>25</v>
       </c>
@@ -2590,12 +2513,11 @@
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="55"/>
-      <c r="S35" s="129"/>
-      <c r="T35" s="130"/>
-      <c r="U35" s="61"/>
-      <c r="V35" s="58"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S35" s="65"/>
+      <c r="T35" s="61"/>
+      <c r="U35" s="58"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="35">
         <v>26</v>
       </c>
@@ -2616,12 +2538,11 @@
       <c r="P36" s="18"/>
       <c r="Q36" s="18"/>
       <c r="R36" s="55"/>
-      <c r="S36" s="129"/>
-      <c r="T36" s="130"/>
-      <c r="U36" s="61"/>
-      <c r="V36" s="58"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S36" s="65"/>
+      <c r="T36" s="61"/>
+      <c r="U36" s="58"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="35">
         <v>27</v>
       </c>
@@ -2642,12 +2563,11 @@
       <c r="P37" s="18"/>
       <c r="Q37" s="18"/>
       <c r="R37" s="55"/>
-      <c r="S37" s="129"/>
-      <c r="T37" s="130"/>
-      <c r="U37" s="61"/>
-      <c r="V37" s="58"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S37" s="65"/>
+      <c r="T37" s="61"/>
+      <c r="U37" s="58"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="35">
         <v>28</v>
       </c>
@@ -2668,12 +2588,11 @@
       <c r="P38" s="18"/>
       <c r="Q38" s="18"/>
       <c r="R38" s="55"/>
-      <c r="S38" s="129"/>
-      <c r="T38" s="130"/>
-      <c r="U38" s="61"/>
-      <c r="V38" s="58"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S38" s="65"/>
+      <c r="T38" s="61"/>
+      <c r="U38" s="58"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="35">
         <v>29</v>
       </c>
@@ -2694,12 +2613,11 @@
       <c r="P39" s="18"/>
       <c r="Q39" s="18"/>
       <c r="R39" s="55"/>
-      <c r="S39" s="129"/>
-      <c r="T39" s="130"/>
-      <c r="U39" s="61"/>
-      <c r="V39" s="58"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S39" s="65"/>
+      <c r="T39" s="61"/>
+      <c r="U39" s="58"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="35">
         <v>30</v>
       </c>
@@ -2720,12 +2638,11 @@
       <c r="P40" s="18"/>
       <c r="Q40" s="18"/>
       <c r="R40" s="55"/>
-      <c r="S40" s="129"/>
-      <c r="T40" s="130"/>
-      <c r="U40" s="61"/>
-      <c r="V40" s="58"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S40" s="65"/>
+      <c r="T40" s="61"/>
+      <c r="U40" s="58"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>31</v>
       </c>
@@ -2746,12 +2663,11 @@
       <c r="P41" s="18"/>
       <c r="Q41" s="18"/>
       <c r="R41" s="55"/>
-      <c r="S41" s="129"/>
-      <c r="T41" s="130"/>
-      <c r="U41" s="61"/>
-      <c r="V41" s="58"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S41" s="65"/>
+      <c r="T41" s="61"/>
+      <c r="U41" s="58"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="35">
         <v>32</v>
       </c>
@@ -2772,12 +2688,11 @@
       <c r="P42" s="18"/>
       <c r="Q42" s="18"/>
       <c r="R42" s="55"/>
-      <c r="S42" s="129"/>
-      <c r="T42" s="130"/>
-      <c r="U42" s="61"/>
-      <c r="V42" s="58"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S42" s="65"/>
+      <c r="T42" s="61"/>
+      <c r="U42" s="58"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="35">
         <v>33</v>
       </c>
@@ -2798,12 +2713,11 @@
       <c r="P43" s="18"/>
       <c r="Q43" s="18"/>
       <c r="R43" s="55"/>
-      <c r="S43" s="129"/>
-      <c r="T43" s="130"/>
-      <c r="U43" s="61"/>
-      <c r="V43" s="58"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S43" s="65"/>
+      <c r="T43" s="61"/>
+      <c r="U43" s="58"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="35">
         <v>34</v>
       </c>
@@ -2824,12 +2738,11 @@
       <c r="P44" s="18"/>
       <c r="Q44" s="18"/>
       <c r="R44" s="55"/>
-      <c r="S44" s="129"/>
-      <c r="T44" s="130"/>
-      <c r="U44" s="61"/>
-      <c r="V44" s="58"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S44" s="65"/>
+      <c r="T44" s="61"/>
+      <c r="U44" s="58"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="35">
         <v>35</v>
       </c>
@@ -2850,12 +2763,11 @@
       <c r="P45" s="18"/>
       <c r="Q45" s="18"/>
       <c r="R45" s="55"/>
-      <c r="S45" s="129"/>
-      <c r="T45" s="130"/>
-      <c r="U45" s="61"/>
-      <c r="V45" s="58"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S45" s="65"/>
+      <c r="T45" s="61"/>
+      <c r="U45" s="58"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="35">
         <v>36</v>
       </c>
@@ -2876,12 +2788,11 @@
       <c r="P46" s="18"/>
       <c r="Q46" s="18"/>
       <c r="R46" s="55"/>
-      <c r="S46" s="129"/>
-      <c r="T46" s="130"/>
-      <c r="U46" s="61"/>
-      <c r="V46" s="58"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S46" s="65"/>
+      <c r="T46" s="61"/>
+      <c r="U46" s="58"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="35">
         <v>37</v>
       </c>
@@ -2902,12 +2813,11 @@
       <c r="P47" s="18"/>
       <c r="Q47" s="18"/>
       <c r="R47" s="55"/>
-      <c r="S47" s="129"/>
-      <c r="T47" s="130"/>
-      <c r="U47" s="61"/>
-      <c r="V47" s="58"/>
-    </row>
-    <row r="48" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S47" s="65"/>
+      <c r="T47" s="61"/>
+      <c r="U47" s="58"/>
+    </row>
+    <row r="48" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="36">
         <v>38</v>
       </c>
@@ -2928,275 +2838,260 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="56"/>
-      <c r="S48" s="131"/>
-      <c r="T48" s="132"/>
-      <c r="U48" s="62"/>
-      <c r="V48" s="59"/>
-    </row>
-    <row r="49" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S48" s="66"/>
+      <c r="T48" s="62"/>
+      <c r="U48" s="59"/>
+    </row>
+    <row r="49" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T49" s="32"/>
-      <c r="U49" s="32"/>
-    </row>
-    <row r="50" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="44"/>
-      <c r="B50" s="75" t="s">
+      <c r="B50" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="76"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="81" t="s">
+      <c r="C50" s="108"/>
+      <c r="D50" s="109"/>
+      <c r="E50" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="81" t="s">
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="I50" s="98"/>
-      <c r="J50" s="82" t="s">
+      <c r="I50" s="96"/>
+      <c r="J50" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K50" s="82"/>
-      <c r="L50" s="81" t="s">
+      <c r="K50" s="110"/>
+      <c r="L50" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="M50" s="82"/>
-      <c r="N50" s="82"/>
-      <c r="O50" s="82"/>
-      <c r="P50" s="119" t="s">
+      <c r="M50" s="110"/>
+      <c r="N50" s="110"/>
+      <c r="O50" s="110"/>
+      <c r="P50" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="Q50" s="120"/>
-      <c r="R50" s="120"/>
-      <c r="S50" s="121"/>
-      <c r="T50" s="116" t="s">
-        <v>31</v>
-      </c>
-      <c r="U50" s="117"/>
-      <c r="V50" s="118"/>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q50" s="103"/>
+      <c r="R50" s="103"/>
+      <c r="S50" s="104"/>
+      <c r="T50" s="100"/>
+      <c r="U50" s="101"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="41">
         <v>1</v>
       </c>
-      <c r="B51" s="103"/>
-      <c r="C51" s="104"/>
-      <c r="D51" s="105"/>
-      <c r="E51" s="83"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="84"/>
-      <c r="H51" s="103"/>
-      <c r="I51" s="105"/>
-      <c r="J51" s="104"/>
-      <c r="K51" s="105"/>
-      <c r="L51" s="103"/>
-      <c r="M51" s="104"/>
-      <c r="N51" s="104"/>
-      <c r="O51" s="104"/>
-      <c r="P51" s="122"/>
-      <c r="Q51" s="123"/>
-      <c r="R51" s="123"/>
-      <c r="S51" s="124"/>
-      <c r="T51" s="125"/>
+      <c r="B51" s="113"/>
+      <c r="C51" s="111"/>
+      <c r="D51" s="112"/>
+      <c r="E51" s="114"/>
+      <c r="F51" s="115"/>
+      <c r="G51" s="115"/>
+      <c r="H51" s="113"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="111"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="113"/>
+      <c r="M51" s="111"/>
+      <c r="N51" s="111"/>
+      <c r="O51" s="111"/>
+      <c r="P51" s="124"/>
+      <c r="Q51" s="125"/>
+      <c r="R51" s="125"/>
+      <c r="S51" s="126"/>
+      <c r="T51" s="127"/>
       <c r="U51" s="126"/>
-      <c r="V51" s="124"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="42">
         <v>2</v>
       </c>
-      <c r="B52" s="78"/>
-      <c r="C52" s="79"/>
-      <c r="D52" s="80"/>
-      <c r="E52" s="85"/>
-      <c r="F52" s="86"/>
-      <c r="G52" s="86"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="80"/>
-      <c r="J52" s="79"/>
-      <c r="K52" s="80"/>
-      <c r="L52" s="78"/>
-      <c r="M52" s="79"/>
-      <c r="N52" s="79"/>
-      <c r="O52" s="79"/>
-      <c r="P52" s="110"/>
-      <c r="Q52" s="111"/>
-      <c r="R52" s="111"/>
-      <c r="S52" s="112"/>
-      <c r="T52" s="115"/>
-      <c r="U52" s="79"/>
-      <c r="V52" s="112"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B52" s="86"/>
+      <c r="C52" s="83"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="69"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="86"/>
+      <c r="I52" s="84"/>
+      <c r="J52" s="83"/>
+      <c r="K52" s="84"/>
+      <c r="L52" s="86"/>
+      <c r="M52" s="83"/>
+      <c r="N52" s="83"/>
+      <c r="O52" s="83"/>
+      <c r="P52" s="119"/>
+      <c r="Q52" s="120"/>
+      <c r="R52" s="120"/>
+      <c r="S52" s="121"/>
+      <c r="T52" s="83"/>
+      <c r="U52" s="121"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="42">
         <v>3</v>
       </c>
-      <c r="B53" s="78"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="80"/>
-      <c r="E53" s="85"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
-      <c r="H53" s="78"/>
-      <c r="I53" s="80"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="80"/>
-      <c r="L53" s="78"/>
-      <c r="M53" s="79"/>
-      <c r="N53" s="79"/>
-      <c r="O53" s="79"/>
-      <c r="P53" s="110"/>
-      <c r="Q53" s="111"/>
-      <c r="R53" s="111"/>
-      <c r="S53" s="112"/>
-      <c r="T53" s="115"/>
-      <c r="U53" s="79"/>
-      <c r="V53" s="112"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B53" s="86"/>
+      <c r="C53" s="83"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="68"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="86"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="83"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="86"/>
+      <c r="M53" s="83"/>
+      <c r="N53" s="83"/>
+      <c r="O53" s="83"/>
+      <c r="P53" s="119"/>
+      <c r="Q53" s="120"/>
+      <c r="R53" s="120"/>
+      <c r="S53" s="121"/>
+      <c r="T53" s="83"/>
+      <c r="U53" s="121"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="42">
         <v>4</v>
       </c>
-      <c r="B54" s="78"/>
-      <c r="C54" s="79"/>
-      <c r="D54" s="80"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="86"/>
-      <c r="G54" s="86"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="80"/>
-      <c r="J54" s="79"/>
-      <c r="K54" s="80"/>
-      <c r="L54" s="78"/>
-      <c r="M54" s="79"/>
-      <c r="N54" s="79"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="110"/>
-      <c r="Q54" s="111"/>
-      <c r="R54" s="111"/>
-      <c r="S54" s="112"/>
-      <c r="T54" s="115"/>
-      <c r="U54" s="79"/>
-      <c r="V54" s="112"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B54" s="86"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="68"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="86"/>
+      <c r="I54" s="84"/>
+      <c r="J54" s="83"/>
+      <c r="K54" s="84"/>
+      <c r="L54" s="86"/>
+      <c r="M54" s="83"/>
+      <c r="N54" s="83"/>
+      <c r="O54" s="83"/>
+      <c r="P54" s="119"/>
+      <c r="Q54" s="120"/>
+      <c r="R54" s="120"/>
+      <c r="S54" s="121"/>
+      <c r="T54" s="83"/>
+      <c r="U54" s="121"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="42">
         <v>5</v>
       </c>
-      <c r="B55" s="78"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="80"/>
-      <c r="E55" s="85"/>
-      <c r="F55" s="86"/>
-      <c r="G55" s="86"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="80"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="80"/>
-      <c r="L55" s="78"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="110"/>
-      <c r="Q55" s="111"/>
-      <c r="R55" s="111"/>
-      <c r="S55" s="112"/>
-      <c r="T55" s="115"/>
-      <c r="U55" s="79"/>
-      <c r="V55" s="112"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B55" s="86"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
+      <c r="H55" s="86"/>
+      <c r="I55" s="84"/>
+      <c r="J55" s="83"/>
+      <c r="K55" s="84"/>
+      <c r="L55" s="86"/>
+      <c r="M55" s="83"/>
+      <c r="N55" s="83"/>
+      <c r="O55" s="83"/>
+      <c r="P55" s="119"/>
+      <c r="Q55" s="120"/>
+      <c r="R55" s="120"/>
+      <c r="S55" s="121"/>
+      <c r="T55" s="83"/>
+      <c r="U55" s="121"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="42">
         <v>6</v>
       </c>
-      <c r="B56" s="78"/>
-      <c r="C56" s="79"/>
-      <c r="D56" s="80"/>
-      <c r="E56" s="85"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="86"/>
-      <c r="H56" s="78"/>
-      <c r="I56" s="80"/>
-      <c r="J56" s="79"/>
-      <c r="K56" s="80"/>
-      <c r="L56" s="78"/>
-      <c r="M56" s="79"/>
-      <c r="N56" s="79"/>
-      <c r="O56" s="79"/>
-      <c r="P56" s="110"/>
-      <c r="Q56" s="111"/>
-      <c r="R56" s="111"/>
-      <c r="S56" s="112"/>
-      <c r="T56" s="115"/>
-      <c r="U56" s="79"/>
-      <c r="V56" s="112"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B56" s="86"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="68"/>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="86"/>
+      <c r="I56" s="84"/>
+      <c r="J56" s="83"/>
+      <c r="K56" s="84"/>
+      <c r="L56" s="86"/>
+      <c r="M56" s="83"/>
+      <c r="N56" s="83"/>
+      <c r="O56" s="83"/>
+      <c r="P56" s="119"/>
+      <c r="Q56" s="120"/>
+      <c r="R56" s="120"/>
+      <c r="S56" s="121"/>
+      <c r="T56" s="83"/>
+      <c r="U56" s="121"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="42">
         <v>7</v>
       </c>
-      <c r="B57" s="78"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="80"/>
-      <c r="E57" s="85"/>
-      <c r="F57" s="86"/>
-      <c r="G57" s="86"/>
-      <c r="H57" s="78"/>
-      <c r="I57" s="80"/>
-      <c r="J57" s="79"/>
-      <c r="K57" s="80"/>
-      <c r="L57" s="78"/>
-      <c r="M57" s="79"/>
-      <c r="N57" s="79"/>
-      <c r="O57" s="79"/>
-      <c r="P57" s="110"/>
-      <c r="Q57" s="111"/>
-      <c r="R57" s="111"/>
-      <c r="S57" s="112"/>
-      <c r="T57" s="115"/>
-      <c r="U57" s="79"/>
-      <c r="V57" s="112"/>
-    </row>
-    <row r="58" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="86"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="86"/>
+      <c r="I57" s="84"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="84"/>
+      <c r="L57" s="86"/>
+      <c r="M57" s="83"/>
+      <c r="N57" s="83"/>
+      <c r="O57" s="83"/>
+      <c r="P57" s="119"/>
+      <c r="Q57" s="120"/>
+      <c r="R57" s="120"/>
+      <c r="S57" s="121"/>
+      <c r="T57" s="83"/>
+      <c r="U57" s="121"/>
+    </row>
+    <row r="58" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="43">
         <v>8</v>
       </c>
-      <c r="B58" s="87"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="102"/>
-      <c r="E58" s="106"/>
-      <c r="F58" s="107"/>
-      <c r="G58" s="107"/>
-      <c r="H58" s="87"/>
-      <c r="I58" s="102"/>
-      <c r="J58" s="88"/>
-      <c r="K58" s="102"/>
-      <c r="L58" s="87"/>
-      <c r="M58" s="88"/>
-      <c r="N58" s="88"/>
-      <c r="O58" s="88"/>
-      <c r="P58" s="113"/>
-      <c r="Q58" s="114"/>
-      <c r="R58" s="114"/>
-      <c r="S58" s="109"/>
-      <c r="T58" s="108"/>
-      <c r="U58" s="88"/>
-      <c r="V58" s="109"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B58" s="81"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="116"/>
+      <c r="F58" s="117"/>
+      <c r="G58" s="117"/>
+      <c r="H58" s="81"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="82"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="81"/>
+      <c r="M58" s="82"/>
+      <c r="N58" s="82"/>
+      <c r="O58" s="82"/>
+      <c r="P58" s="122"/>
+      <c r="Q58" s="123"/>
+      <c r="R58" s="123"/>
+      <c r="S58" s="118"/>
+      <c r="T58" s="82"/>
+      <c r="U58" s="118"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="32"/>
       <c r="T59" s="32"/>
-      <c r="U59" s="32"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B60" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C60" s="1"/>
       <c r="T60" s="32"/>
-      <c r="U60" s="32"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B61" s="32" t="s">
         <v>20</v>
       </c>
@@ -3212,18 +3107,16 @@
       <c r="L61" s="38"/>
       <c r="M61" s="38"/>
       <c r="T61" s="32"/>
-      <c r="U61" s="32"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B63" s="39" t="s">
         <v>7</v>
       </c>
       <c r="T63" s="32"/>
-      <c r="U63" s="32"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B64" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" s="40"/>
       <c r="D64" s="37"/>
@@ -3243,9 +3136,8 @@
       <c r="R64" s="37"/>
       <c r="S64" s="37"/>
       <c r="T64" s="32"/>
-      <c r="U64" s="32"/>
-    </row>
-    <row r="65" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E65" s="38"/>
       <c r="F65" s="38"/>
       <c r="G65" s="38"/>
@@ -3256,105 +3148,29 @@
       <c r="L65" s="38"/>
       <c r="M65" s="38"/>
       <c r="T65" s="32"/>
-      <c r="U65" s="32"/>
-    </row>
-    <row r="66" spans="5:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="5:20" x14ac:dyDescent="0.25">
       <c r="T66" s="32"/>
-      <c r="U66" s="32"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QsiFAyxPtOQZ41DNyRWA27VkKi1BharO+Q9MPQoeCPndrYLfA5Sge1poB8UR4EluX12Rrn2D0qwqzrMQWCW12Q==" saltValue="2s+P0spzHtLpNmBZs4NoLA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="112">
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S39:T39"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S46:T46"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="L55:O55"/>
-    <mergeCell ref="L56:O56"/>
-    <mergeCell ref="L57:O57"/>
-    <mergeCell ref="T50:V50"/>
-    <mergeCell ref="P50:S50"/>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="74">
     <mergeCell ref="P51:S51"/>
     <mergeCell ref="P52:S52"/>
     <mergeCell ref="P53:S53"/>
-    <mergeCell ref="T51:V51"/>
-    <mergeCell ref="T52:V52"/>
-    <mergeCell ref="T53:V53"/>
-    <mergeCell ref="T58:V58"/>
+    <mergeCell ref="T51:U51"/>
+    <mergeCell ref="T52:U52"/>
+    <mergeCell ref="T53:U53"/>
+    <mergeCell ref="T58:U58"/>
     <mergeCell ref="P54:S54"/>
     <mergeCell ref="P55:S55"/>
     <mergeCell ref="P56:S56"/>
     <mergeCell ref="P57:S57"/>
     <mergeCell ref="P58:S58"/>
-    <mergeCell ref="T54:V54"/>
-    <mergeCell ref="T55:V55"/>
-    <mergeCell ref="T56:V56"/>
-    <mergeCell ref="T57:V57"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="L58:O58"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="C7:R7"/>
-    <mergeCell ref="S9:T10"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="T54:U54"/>
+    <mergeCell ref="T55:U55"/>
+    <mergeCell ref="T56:U56"/>
+    <mergeCell ref="T57:U57"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
@@ -3363,20 +3179,56 @@
     <mergeCell ref="E56:G56"/>
     <mergeCell ref="E57:G57"/>
     <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="L55:O55"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="C7:R7"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="T50:U50"/>
+    <mergeCell ref="P50:S50"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:O50"/>
+    <mergeCell ref="L58:O58"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L56:O56"/>
+    <mergeCell ref="L57:O57"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations xWindow="727" yWindow="303" count="13">
@@ -3389,7 +3241,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Отметка должна состоять из неповторяющегося номера солистки и РУССКОЙ буквы С в конце." sqref="O11:O48 I11:I48" xr:uid="{F34D888B-FB3D-49A1-B31A-72D03D5EC925}">
       <formula1>AND(ISNUMBER(_xlfn.NUMBERVALUE(LEFT(I11,1))),RIGHT(I11,1)="С")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Отметка должна состоять из неповторяющегося номера группы и букв Г или Р (для резерва)." sqref="R11:R48 L11:M48" xr:uid="{68FA2C25-0C13-4959-930C-70F2F8A568BC}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Отметка должна состоять из неповторяющегося номера группы и букв Г или Р (для резерва)." sqref="R11:R48 L11:M48 N11:N22" xr:uid="{68FA2C25-0C13-4959-930C-70F2F8A568BC}">
       <formula1>AND(ISNUMBER(_xlfn.NUMBERVALUE(LEFT(L11,1))),OR(RIGHT(L11,1)="Г",RIGHT(L11,1)="Р"))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Представитель команды должен быть единственным человеком, отмеченным русской буквой П." sqref="E51:G58" xr:uid="{FF1574E9-7D0B-4A82-9EE4-9482CC0B8609}">
@@ -3416,8 +3268,8 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="G11:G48" xr:uid="{95FD4B4C-7AC9-4C5B-A1CF-87F7AB7247B7}">
       <formula1>AND(YEAR(TODAY())&gt;YEAR(C11)+14,YEAR(TODAY())&lt;YEAR(C11)+19,G11="+")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Отметка должна состоять из неповторяющегося номера группы и букв К или Р (для резерва)." sqref="N11:N48" xr:uid="{3D0A0695-8181-41AB-89A0-470CB56D71C2}">
-      <formula1>AND(ISNUMBER(_xlfn.NUMBERVALUE(LEFT(N11,1))),OR(RIGHT(N11,1)="К",RIGHT(N11,1)="Р"))</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Отметка должна состоять из неповторяющегося номера группы и букв К или Р (для резерва)." sqref="N23:N48" xr:uid="{3D0A0695-8181-41AB-89A0-470CB56D71C2}">
+      <formula1>AND(ISNUMBER(_xlfn.NUMBERVALUE(LEFT(N23,1))),OR(RIGHT(N23,1)="К",RIGHT(N23,1)="Р"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Fixed dob in sportsmen list;
</commit_message>
<xml_diff>
--- a/assets/Заявка.xlsx
+++ b/assets/Заявка.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Игорь\WebstormProjects\synchroreg\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2E8D49-7101-46FD-9112-6EF55C08BB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF7FF91-257F-4DDA-AA92-90ACFC39BB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2430" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заявка" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>ТЕХНИЧЕСКАЯ ЗАЯВКА</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Общество/Школа</t>
   </si>
   <si>
-    <t>&gt;18</t>
-  </si>
-  <si>
     <t>Соло</t>
   </si>
   <si>
@@ -151,6 +148,12 @@
   </si>
   <si>
     <t>Приказ о продлении категории</t>
+  </si>
+  <si>
+    <t>qe</t>
+  </si>
+  <si>
+    <t>&gt;15</t>
   </si>
 </sst>
 </file>
@@ -1110,163 +1113,12 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1303,15 +1155,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1340,33 +1183,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1381,18 +1197,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1407,6 +1211,205 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1751,198 +1754,200 @@
   <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="20" style="75" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="75" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="76" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="76" customWidth="1"/>
-    <col min="6" max="6" width="10" style="75" customWidth="1"/>
-    <col min="7" max="7" width="5" style="75" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="75" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="75" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="75" customWidth="1"/>
-    <col min="11" max="12" width="6.140625" style="75" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="75" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="75" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="75" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" style="75" customWidth="1"/>
-    <col min="17" max="17" width="5.85546875" style="75" customWidth="1"/>
-    <col min="18" max="18" width="6" style="75" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" style="75" customWidth="1"/>
-    <col min="20" max="20" width="8" style="75" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" style="75" customWidth="1"/>
+    <col min="2" max="2" width="20" style="48" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="49" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="49" customWidth="1"/>
+    <col min="6" max="6" width="10" style="48" customWidth="1"/>
+    <col min="7" max="7" width="5" style="48" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="48" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="48" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="48" customWidth="1"/>
+    <col min="11" max="12" width="6.140625" style="48" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="48" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="48" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="48" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="48" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" style="48" customWidth="1"/>
+    <col min="18" max="18" width="6" style="48" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" style="48" customWidth="1"/>
+    <col min="20" max="20" width="8" style="48" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" style="48" customWidth="1"/>
     <col min="22" max="22" width="18.42578125" customWidth="1"/>
-    <col min="23" max="23" width="23.140625" style="75" customWidth="1"/>
+    <col min="23" max="23" width="23.140625" style="48" customWidth="1"/>
     <col min="24" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="47" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="74"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="74"/>
+      <c r="E4" s="47"/>
     </row>
     <row r="5" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="74"/>
+      <c r="E5" s="47"/>
     </row>
     <row r="7" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="71"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="118"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="118"/>
     </row>
     <row r="8" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="130" t="s">
+      <c r="B9" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="105"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="107" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="109" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="111" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="112"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="125" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="126"/>
+      <c r="M9" s="126"/>
+      <c r="N9" s="126"/>
+      <c r="O9" s="126"/>
+      <c r="P9" s="127"/>
+      <c r="Q9" s="128" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="129"/>
+      <c r="S9" s="129"/>
+      <c r="T9" s="130"/>
+      <c r="U9" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="V9" s="90" t="s">
         <v>31</v>
-      </c>
-      <c r="F9" s="131" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="87" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" s="88"/>
-      <c r="S9" s="88"/>
-      <c r="T9" s="89"/>
-      <c r="U9" s="90" t="s">
-        <v>21</v>
-      </c>
-      <c r="V9" s="91" t="s">
-        <v>32</v>
       </c>
       <c r="W9" s="92" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="26" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="73"/>
-      <c r="B10" s="93" t="s">
+      <c r="A10" s="103"/>
+      <c r="B10" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="D10" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="95" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="132"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="96" t="s">
+      <c r="E10" s="108"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="97" t="s">
+      <c r="I10" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="98" t="s">
+      <c r="J10" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="99" t="s">
+      <c r="L10" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="100" t="s">
+      <c r="M10" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="100" t="s">
+      <c r="N10" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="100" t="s">
+      <c r="O10" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="100" t="s">
+      <c r="P10" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="101" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q10" s="102" t="s">
+      <c r="Q10" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="103" t="s">
+      <c r="S10" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="S10" s="103" t="s">
+      <c r="T10" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="T10" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="U10" s="105"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="107"/>
+      <c r="U10" s="117"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="93"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>1</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="C11" s="46"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="111"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="43"/>
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
@@ -1957,10 +1962,10 @@
       <c r="Q11" s="10"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
-      <c r="T11" s="134"/>
-      <c r="U11" s="128"/>
+      <c r="T11" s="76"/>
+      <c r="U11" s="74"/>
       <c r="V11" s="37"/>
-      <c r="W11" s="135"/>
+      <c r="W11" s="77"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
@@ -1968,8 +1973,8 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="42"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="111"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="43"/>
       <c r="G12" s="12"/>
       <c r="H12" s="13"/>
@@ -1984,10 +1989,10 @@
       <c r="Q12" s="17"/>
       <c r="R12" s="18"/>
       <c r="S12" s="18"/>
-      <c r="T12" s="136"/>
-      <c r="U12" s="110"/>
+      <c r="T12" s="78"/>
+      <c r="U12" s="65"/>
       <c r="V12" s="38"/>
-      <c r="W12" s="137"/>
+      <c r="W12" s="79"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
@@ -1995,8 +2000,8 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="42"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="111"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="43"/>
       <c r="G13" s="12"/>
       <c r="H13" s="13"/>
@@ -2011,10 +2016,10 @@
       <c r="Q13" s="17"/>
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
-      <c r="T13" s="136"/>
-      <c r="U13" s="110"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="65"/>
       <c r="V13" s="38"/>
-      <c r="W13" s="137"/>
+      <c r="W13" s="79"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
@@ -2022,8 +2027,8 @@
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="42"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="111"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="66"/>
       <c r="F14" s="43"/>
       <c r="G14" s="12"/>
       <c r="H14" s="13"/>
@@ -2038,10 +2043,10 @@
       <c r="Q14" s="17"/>
       <c r="R14" s="18"/>
       <c r="S14" s="18"/>
-      <c r="T14" s="136"/>
-      <c r="U14" s="110"/>
+      <c r="T14" s="78"/>
+      <c r="U14" s="65"/>
       <c r="V14" s="38"/>
-      <c r="W14" s="137"/>
+      <c r="W14" s="79"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
@@ -2049,8 +2054,8 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="42"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="111"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="66"/>
       <c r="F15" s="43"/>
       <c r="G15" s="12"/>
       <c r="H15" s="13"/>
@@ -2065,10 +2070,10 @@
       <c r="Q15" s="17"/>
       <c r="R15" s="18"/>
       <c r="S15" s="18"/>
-      <c r="T15" s="136"/>
-      <c r="U15" s="110"/>
+      <c r="T15" s="78"/>
+      <c r="U15" s="65"/>
       <c r="V15" s="38"/>
-      <c r="W15" s="137"/>
+      <c r="W15" s="79"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
@@ -2076,8 +2081,8 @@
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="42"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="111"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="66"/>
       <c r="F16" s="43"/>
       <c r="G16" s="12"/>
       <c r="H16" s="13"/>
@@ -2092,10 +2097,10 @@
       <c r="Q16" s="17"/>
       <c r="R16" s="18"/>
       <c r="S16" s="18"/>
-      <c r="T16" s="136"/>
-      <c r="U16" s="110"/>
+      <c r="T16" s="78"/>
+      <c r="U16" s="65"/>
       <c r="V16" s="38"/>
-      <c r="W16" s="137"/>
+      <c r="W16" s="79"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
@@ -2103,8 +2108,8 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="42"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="111"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="66"/>
       <c r="F17" s="43"/>
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
@@ -2119,10 +2124,10 @@
       <c r="Q17" s="17"/>
       <c r="R17" s="18"/>
       <c r="S17" s="18"/>
-      <c r="T17" s="136"/>
-      <c r="U17" s="110"/>
+      <c r="T17" s="78"/>
+      <c r="U17" s="65"/>
       <c r="V17" s="38"/>
-      <c r="W17" s="137"/>
+      <c r="W17" s="79"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
@@ -2130,8 +2135,8 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="42"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="111"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="66"/>
       <c r="F18" s="43"/>
       <c r="G18" s="12"/>
       <c r="H18" s="13"/>
@@ -2146,10 +2151,10 @@
       <c r="Q18" s="17"/>
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="136"/>
-      <c r="U18" s="110"/>
+      <c r="T18" s="78"/>
+      <c r="U18" s="65"/>
       <c r="V18" s="38"/>
-      <c r="W18" s="137"/>
+      <c r="W18" s="79"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
@@ -2157,8 +2162,8 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="42"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="111"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="43"/>
       <c r="G19" s="12"/>
       <c r="H19" s="13"/>
@@ -2173,10 +2178,10 @@
       <c r="Q19" s="17"/>
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
-      <c r="T19" s="136"/>
-      <c r="U19" s="110"/>
+      <c r="T19" s="78"/>
+      <c r="U19" s="65"/>
       <c r="V19" s="38"/>
-      <c r="W19" s="137"/>
+      <c r="W19" s="79"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
@@ -2184,8 +2189,8 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="42"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="111"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="66"/>
       <c r="F20" s="43"/>
       <c r="G20" s="12"/>
       <c r="H20" s="13"/>
@@ -2200,10 +2205,10 @@
       <c r="Q20" s="17"/>
       <c r="R20" s="18"/>
       <c r="S20" s="18"/>
-      <c r="T20" s="136"/>
-      <c r="U20" s="110"/>
+      <c r="T20" s="78"/>
+      <c r="U20" s="65"/>
       <c r="V20" s="38"/>
-      <c r="W20" s="137"/>
+      <c r="W20" s="79"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
@@ -2211,8 +2216,8 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="42"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="111"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="43"/>
       <c r="G21" s="12"/>
       <c r="H21" s="13"/>
@@ -2227,10 +2232,10 @@
       <c r="Q21" s="17"/>
       <c r="R21" s="18"/>
       <c r="S21" s="18"/>
-      <c r="T21" s="136"/>
-      <c r="U21" s="110"/>
+      <c r="T21" s="78"/>
+      <c r="U21" s="65"/>
       <c r="V21" s="38"/>
-      <c r="W21" s="137"/>
+      <c r="W21" s="79"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
@@ -2238,8 +2243,8 @@
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="42"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="111"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="66"/>
       <c r="F22" s="43"/>
       <c r="G22" s="12"/>
       <c r="H22" s="13"/>
@@ -2254,10 +2259,10 @@
       <c r="Q22" s="17"/>
       <c r="R22" s="18"/>
       <c r="S22" s="18"/>
-      <c r="T22" s="136"/>
-      <c r="U22" s="110"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="65"/>
       <c r="V22" s="38"/>
-      <c r="W22" s="137"/>
+      <c r="W22" s="79"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
@@ -2265,8 +2270,8 @@
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="42"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="111"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="66"/>
       <c r="F23" s="43"/>
       <c r="G23" s="12"/>
       <c r="H23" s="13"/>
@@ -2277,12 +2282,12 @@
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
-      <c r="P23" s="112"/>
+      <c r="P23" s="67"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="18"/>
       <c r="S23" s="18"/>
       <c r="T23" s="33"/>
-      <c r="U23" s="110"/>
+      <c r="U23" s="65"/>
       <c r="V23" s="38"/>
       <c r="W23" s="35"/>
     </row>
@@ -2292,8 +2297,8 @@
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="111"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="43"/>
       <c r="G24" s="12"/>
       <c r="H24" s="13"/>
@@ -2304,12 +2309,12 @@
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
-      <c r="P24" s="112"/>
+      <c r="P24" s="67"/>
       <c r="Q24" s="17"/>
       <c r="R24" s="18"/>
       <c r="S24" s="18"/>
       <c r="T24" s="33"/>
-      <c r="U24" s="110"/>
+      <c r="U24" s="65"/>
       <c r="V24" s="38"/>
       <c r="W24" s="35"/>
     </row>
@@ -2319,8 +2324,8 @@
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="111"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="66"/>
       <c r="F25" s="43"/>
       <c r="G25" s="12"/>
       <c r="H25" s="13"/>
@@ -2331,12 +2336,12 @@
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
-      <c r="P25" s="112"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="17"/>
       <c r="R25" s="18"/>
       <c r="S25" s="18"/>
       <c r="T25" s="33"/>
-      <c r="U25" s="110"/>
+      <c r="U25" s="65"/>
       <c r="V25" s="38"/>
       <c r="W25" s="35"/>
     </row>
@@ -2346,8 +2351,8 @@
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="42"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="111"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="66"/>
       <c r="F26" s="43"/>
       <c r="G26" s="12"/>
       <c r="H26" s="13"/>
@@ -2358,12 +2363,12 @@
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
-      <c r="P26" s="112"/>
+      <c r="P26" s="67"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
       <c r="T26" s="33"/>
-      <c r="U26" s="110"/>
+      <c r="U26" s="65"/>
       <c r="V26" s="38"/>
       <c r="W26" s="35"/>
     </row>
@@ -2373,8 +2378,8 @@
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="42"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="111"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="66"/>
       <c r="F27" s="43"/>
       <c r="G27" s="12"/>
       <c r="H27" s="13"/>
@@ -2385,12 +2390,12 @@
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
-      <c r="P27" s="112"/>
+      <c r="P27" s="67"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="18"/>
       <c r="S27" s="18"/>
       <c r="T27" s="33"/>
-      <c r="U27" s="110"/>
+      <c r="U27" s="65"/>
       <c r="V27" s="38"/>
       <c r="W27" s="35"/>
     </row>
@@ -2400,8 +2405,8 @@
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="111"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="66"/>
       <c r="F28" s="43"/>
       <c r="G28" s="12"/>
       <c r="H28" s="13"/>
@@ -2412,12 +2417,12 @@
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
-      <c r="P28" s="112"/>
+      <c r="P28" s="67"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="18"/>
       <c r="S28" s="18"/>
       <c r="T28" s="33"/>
-      <c r="U28" s="110"/>
+      <c r="U28" s="65"/>
       <c r="V28" s="38"/>
       <c r="W28" s="35"/>
     </row>
@@ -2427,8 +2432,8 @@
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="42"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="111"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="66"/>
       <c r="F29" s="43"/>
       <c r="G29" s="12"/>
       <c r="H29" s="13"/>
@@ -2439,12 +2444,12 @@
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
       <c r="O29" s="16"/>
-      <c r="P29" s="112"/>
+      <c r="P29" s="67"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="18"/>
       <c r="S29" s="18"/>
       <c r="T29" s="33"/>
-      <c r="U29" s="110"/>
+      <c r="U29" s="65"/>
       <c r="V29" s="38"/>
       <c r="W29" s="35"/>
     </row>
@@ -2454,8 +2459,8 @@
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="42"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="111"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="66"/>
       <c r="F30" s="43"/>
       <c r="G30" s="12"/>
       <c r="H30" s="13"/>
@@ -2466,12 +2471,12 @@
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
       <c r="O30" s="16"/>
-      <c r="P30" s="112"/>
+      <c r="P30" s="67"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="18"/>
       <c r="S30" s="18"/>
       <c r="T30" s="33"/>
-      <c r="U30" s="110"/>
+      <c r="U30" s="65"/>
       <c r="V30" s="38"/>
       <c r="W30" s="35"/>
     </row>
@@ -2481,8 +2486,8 @@
       </c>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
-      <c r="D31" s="109"/>
-      <c r="E31" s="111"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="66"/>
       <c r="F31" s="43"/>
       <c r="G31" s="12"/>
       <c r="H31" s="13"/>
@@ -2493,12 +2498,12 @@
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
-      <c r="P31" s="112"/>
+      <c r="P31" s="67"/>
       <c r="Q31" s="17"/>
       <c r="R31" s="18"/>
       <c r="S31" s="18"/>
       <c r="T31" s="33"/>
-      <c r="U31" s="110"/>
+      <c r="U31" s="65"/>
       <c r="V31" s="38"/>
       <c r="W31" s="35"/>
     </row>
@@ -2508,8 +2513,8 @@
       </c>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
-      <c r="D32" s="109"/>
-      <c r="E32" s="111"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="66"/>
       <c r="F32" s="43"/>
       <c r="G32" s="12"/>
       <c r="H32" s="13"/>
@@ -2520,12 +2525,12 @@
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
-      <c r="P32" s="112"/>
+      <c r="P32" s="67"/>
       <c r="Q32" s="17"/>
       <c r="R32" s="18"/>
       <c r="S32" s="18"/>
       <c r="T32" s="33"/>
-      <c r="U32" s="110"/>
+      <c r="U32" s="65"/>
       <c r="V32" s="38"/>
       <c r="W32" s="35"/>
     </row>
@@ -2535,8 +2540,8 @@
       </c>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="111"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="66"/>
       <c r="F33" s="43"/>
       <c r="G33" s="12"/>
       <c r="H33" s="13"/>
@@ -2547,12 +2552,12 @@
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
-      <c r="P33" s="112"/>
+      <c r="P33" s="67"/>
       <c r="Q33" s="17"/>
       <c r="R33" s="18"/>
       <c r="S33" s="18"/>
       <c r="T33" s="33"/>
-      <c r="U33" s="110"/>
+      <c r="U33" s="65"/>
       <c r="V33" s="38"/>
       <c r="W33" s="35"/>
     </row>
@@ -2562,8 +2567,8 @@
       </c>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="111"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="66"/>
       <c r="F34" s="43"/>
       <c r="G34" s="12"/>
       <c r="H34" s="13"/>
@@ -2574,12 +2579,12 @@
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
-      <c r="P34" s="112"/>
+      <c r="P34" s="67"/>
       <c r="Q34" s="17"/>
       <c r="R34" s="18"/>
       <c r="S34" s="18"/>
       <c r="T34" s="33"/>
-      <c r="U34" s="110"/>
+      <c r="U34" s="65"/>
       <c r="V34" s="38"/>
       <c r="W34" s="35"/>
     </row>
@@ -2589,8 +2594,8 @@
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
-      <c r="D35" s="109"/>
-      <c r="E35" s="111"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="66"/>
       <c r="F35" s="43"/>
       <c r="G35" s="12"/>
       <c r="H35" s="13"/>
@@ -2601,12 +2606,12 @@
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
-      <c r="P35" s="112"/>
+      <c r="P35" s="67"/>
       <c r="Q35" s="17"/>
       <c r="R35" s="18"/>
       <c r="S35" s="18"/>
       <c r="T35" s="33"/>
-      <c r="U35" s="110"/>
+      <c r="U35" s="65"/>
       <c r="V35" s="38"/>
       <c r="W35" s="35"/>
     </row>
@@ -2616,8 +2621,8 @@
       </c>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
-      <c r="D36" s="109"/>
-      <c r="E36" s="111"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="66"/>
       <c r="F36" s="43"/>
       <c r="G36" s="12"/>
       <c r="H36" s="13"/>
@@ -2628,12 +2633,12 @@
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
-      <c r="P36" s="112"/>
+      <c r="P36" s="67"/>
       <c r="Q36" s="17"/>
       <c r="R36" s="18"/>
       <c r="S36" s="18"/>
       <c r="T36" s="33"/>
-      <c r="U36" s="110"/>
+      <c r="U36" s="65"/>
       <c r="V36" s="38"/>
       <c r="W36" s="35"/>
     </row>
@@ -2643,8 +2648,8 @@
       </c>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
-      <c r="D37" s="109"/>
-      <c r="E37" s="111"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="66"/>
       <c r="F37" s="43"/>
       <c r="G37" s="12"/>
       <c r="H37" s="13"/>
@@ -2655,12 +2660,12 @@
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="112"/>
+      <c r="P37" s="67"/>
       <c r="Q37" s="17"/>
       <c r="R37" s="18"/>
       <c r="S37" s="18"/>
       <c r="T37" s="33"/>
-      <c r="U37" s="110"/>
+      <c r="U37" s="65"/>
       <c r="V37" s="38"/>
       <c r="W37" s="35"/>
     </row>
@@ -2670,8 +2675,8 @@
       </c>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
-      <c r="D38" s="109"/>
-      <c r="E38" s="111"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="66"/>
       <c r="F38" s="43"/>
       <c r="G38" s="12"/>
       <c r="H38" s="13"/>
@@ -2682,12 +2687,12 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="112"/>
+      <c r="P38" s="67"/>
       <c r="Q38" s="17"/>
       <c r="R38" s="18"/>
       <c r="S38" s="18"/>
       <c r="T38" s="33"/>
-      <c r="U38" s="110"/>
+      <c r="U38" s="65"/>
       <c r="V38" s="38"/>
       <c r="W38" s="35"/>
     </row>
@@ -2697,8 +2702,8 @@
       </c>
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="111"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="66"/>
       <c r="F39" s="43"/>
       <c r="G39" s="12"/>
       <c r="H39" s="13"/>
@@ -2709,12 +2714,12 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="112"/>
+      <c r="P39" s="67"/>
       <c r="Q39" s="17"/>
       <c r="R39" s="18"/>
       <c r="S39" s="18"/>
       <c r="T39" s="33"/>
-      <c r="U39" s="110"/>
+      <c r="U39" s="65"/>
       <c r="V39" s="38"/>
       <c r="W39" s="35"/>
     </row>
@@ -2724,8 +2729,8 @@
       </c>
       <c r="B40" s="41"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="109"/>
-      <c r="E40" s="111"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="66"/>
       <c r="F40" s="43"/>
       <c r="G40" s="12"/>
       <c r="H40" s="13"/>
@@ -2736,12 +2741,12 @@
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
-      <c r="P40" s="112"/>
+      <c r="P40" s="67"/>
       <c r="Q40" s="17"/>
       <c r="R40" s="18"/>
       <c r="S40" s="18"/>
       <c r="T40" s="33"/>
-      <c r="U40" s="110"/>
+      <c r="U40" s="65"/>
       <c r="V40" s="38"/>
       <c r="W40" s="35"/>
     </row>
@@ -2751,8 +2756,8 @@
       </c>
       <c r="B41" s="41"/>
       <c r="C41" s="42"/>
-      <c r="D41" s="109"/>
-      <c r="E41" s="111"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="66"/>
       <c r="F41" s="43"/>
       <c r="G41" s="12"/>
       <c r="H41" s="13"/>
@@ -2763,12 +2768,12 @@
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
-      <c r="P41" s="112"/>
+      <c r="P41" s="67"/>
       <c r="Q41" s="17"/>
       <c r="R41" s="18"/>
       <c r="S41" s="18"/>
       <c r="T41" s="33"/>
-      <c r="U41" s="110"/>
+      <c r="U41" s="65"/>
       <c r="V41" s="38"/>
       <c r="W41" s="35"/>
     </row>
@@ -2778,8 +2783,8 @@
       </c>
       <c r="B42" s="41"/>
       <c r="C42" s="42"/>
-      <c r="D42" s="109"/>
-      <c r="E42" s="111"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="66"/>
       <c r="F42" s="43"/>
       <c r="G42" s="12"/>
       <c r="H42" s="13"/>
@@ -2790,12 +2795,12 @@
       <c r="M42" s="16"/>
       <c r="N42" s="16"/>
       <c r="O42" s="16"/>
-      <c r="P42" s="112"/>
+      <c r="P42" s="67"/>
       <c r="Q42" s="17"/>
       <c r="R42" s="18"/>
       <c r="S42" s="18"/>
       <c r="T42" s="33"/>
-      <c r="U42" s="110"/>
+      <c r="U42" s="65"/>
       <c r="V42" s="38"/>
       <c r="W42" s="35"/>
     </row>
@@ -2805,8 +2810,8 @@
       </c>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
-      <c r="D43" s="109"/>
-      <c r="E43" s="111"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="66"/>
       <c r="F43" s="43"/>
       <c r="G43" s="12"/>
       <c r="H43" s="13"/>
@@ -2817,12 +2822,12 @@
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
       <c r="O43" s="16"/>
-      <c r="P43" s="112"/>
+      <c r="P43" s="67"/>
       <c r="Q43" s="17"/>
       <c r="R43" s="18"/>
       <c r="S43" s="18"/>
       <c r="T43" s="33"/>
-      <c r="U43" s="110"/>
+      <c r="U43" s="65"/>
       <c r="V43" s="38"/>
       <c r="W43" s="35"/>
     </row>
@@ -2832,8 +2837,8 @@
       </c>
       <c r="B44" s="41"/>
       <c r="C44" s="42"/>
-      <c r="D44" s="109"/>
-      <c r="E44" s="111"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="66"/>
       <c r="F44" s="43"/>
       <c r="G44" s="12"/>
       <c r="H44" s="13"/>
@@ -2844,12 +2849,12 @@
       <c r="M44" s="16"/>
       <c r="N44" s="16"/>
       <c r="O44" s="16"/>
-      <c r="P44" s="112"/>
+      <c r="P44" s="67"/>
       <c r="Q44" s="17"/>
       <c r="R44" s="18"/>
       <c r="S44" s="18"/>
       <c r="T44" s="33"/>
-      <c r="U44" s="110"/>
+      <c r="U44" s="65"/>
       <c r="V44" s="38"/>
       <c r="W44" s="35"/>
     </row>
@@ -2859,8 +2864,8 @@
       </c>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
-      <c r="D45" s="109"/>
-      <c r="E45" s="111"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="66"/>
       <c r="F45" s="43"/>
       <c r="G45" s="12"/>
       <c r="H45" s="13"/>
@@ -2871,12 +2876,12 @@
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
-      <c r="P45" s="112"/>
+      <c r="P45" s="67"/>
       <c r="Q45" s="17"/>
       <c r="R45" s="18"/>
       <c r="S45" s="18"/>
       <c r="T45" s="33"/>
-      <c r="U45" s="110"/>
+      <c r="U45" s="65"/>
       <c r="V45" s="38"/>
       <c r="W45" s="35"/>
     </row>
@@ -2886,8 +2891,8 @@
       </c>
       <c r="B46" s="41"/>
       <c r="C46" s="42"/>
-      <c r="D46" s="109"/>
-      <c r="E46" s="111"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="66"/>
       <c r="F46" s="43"/>
       <c r="G46" s="12"/>
       <c r="H46" s="13"/>
@@ -2898,12 +2903,12 @@
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
-      <c r="P46" s="112"/>
+      <c r="P46" s="67"/>
       <c r="Q46" s="17"/>
       <c r="R46" s="18"/>
       <c r="S46" s="18"/>
       <c r="T46" s="33"/>
-      <c r="U46" s="110"/>
+      <c r="U46" s="65"/>
       <c r="V46" s="38"/>
       <c r="W46" s="35"/>
     </row>
@@ -2913,8 +2918,8 @@
       </c>
       <c r="B47" s="41"/>
       <c r="C47" s="42"/>
-      <c r="D47" s="109"/>
-      <c r="E47" s="111"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="66"/>
       <c r="F47" s="43"/>
       <c r="G47" s="12"/>
       <c r="H47" s="13"/>
@@ -2925,12 +2930,12 @@
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
       <c r="O47" s="16"/>
-      <c r="P47" s="112"/>
+      <c r="P47" s="67"/>
       <c r="Q47" s="17"/>
       <c r="R47" s="18"/>
       <c r="S47" s="18"/>
       <c r="T47" s="33"/>
-      <c r="U47" s="110"/>
+      <c r="U47" s="65"/>
       <c r="V47" s="38"/>
       <c r="W47" s="35"/>
     </row>
@@ -2940,8 +2945,8 @@
       </c>
       <c r="B48" s="44"/>
       <c r="C48" s="45"/>
-      <c r="D48" s="113"/>
-      <c r="E48" s="114"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="69"/>
       <c r="F48" s="40"/>
       <c r="G48" s="19"/>
       <c r="H48" s="20"/>
@@ -2952,346 +2957,330 @@
       <c r="M48" s="23"/>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
-      <c r="P48" s="115"/>
+      <c r="P48" s="70"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
       <c r="T48" s="34"/>
-      <c r="U48" s="129"/>
+      <c r="U48" s="75"/>
       <c r="V48" s="39"/>
       <c r="W48" s="36"/>
     </row>
     <row r="49" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="V49" s="76"/>
+      <c r="V49" s="49"/>
     </row>
     <row r="50" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="32"/>
-      <c r="B50" s="116" t="s">
+      <c r="B50" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="117"/>
-      <c r="D50" s="118"/>
+      <c r="C50" s="122"/>
+      <c r="D50" s="123"/>
       <c r="E50" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="120"/>
-      <c r="G50" s="120"/>
+      <c r="F50" s="124"/>
+      <c r="G50" s="124"/>
       <c r="H50" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="I50" s="121"/>
-      <c r="J50" s="120" t="s">
+      <c r="I50" s="120"/>
+      <c r="J50" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="K50" s="120"/>
+      <c r="K50" s="124"/>
       <c r="L50" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="M50" s="124"/>
+      <c r="N50" s="124"/>
+      <c r="O50" s="124"/>
+      <c r="P50" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="M50" s="120"/>
-      <c r="N50" s="120"/>
-      <c r="O50" s="120"/>
-      <c r="P50" s="122" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q50" s="123"/>
-      <c r="R50" s="123"/>
-      <c r="S50" s="123"/>
-      <c r="T50" s="124"/>
-      <c r="U50" s="122" t="s">
-        <v>38</v>
-      </c>
-      <c r="V50" s="123"/>
+      <c r="Q50" s="95"/>
+      <c r="R50" s="95"/>
+      <c r="S50" s="95"/>
+      <c r="T50" s="96"/>
+      <c r="U50" s="94" t="s">
+        <v>37</v>
+      </c>
+      <c r="V50" s="95"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="29">
         <v>1</v>
       </c>
-      <c r="B51" s="62"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="63"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="62"/>
-      <c r="M51" s="63"/>
-      <c r="N51" s="63"/>
-      <c r="O51" s="63"/>
-      <c r="P51" s="47"/>
-      <c r="Q51" s="48"/>
-      <c r="R51" s="48"/>
-      <c r="S51" s="48"/>
-      <c r="T51" s="49"/>
-      <c r="U51" s="63"/>
-      <c r="V51" s="64"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="100"/>
+      <c r="D51" s="101"/>
+      <c r="E51" s="132"/>
+      <c r="F51" s="133"/>
+      <c r="G51" s="133"/>
+      <c r="H51" s="131"/>
+      <c r="I51" s="101"/>
+      <c r="J51" s="100"/>
+      <c r="K51" s="101"/>
+      <c r="L51" s="131"/>
+      <c r="M51" s="100"/>
+      <c r="N51" s="100"/>
+      <c r="O51" s="100"/>
+      <c r="P51" s="97"/>
+      <c r="Q51" s="98"/>
+      <c r="R51" s="98"/>
+      <c r="S51" s="98"/>
+      <c r="T51" s="99"/>
+      <c r="U51" s="100"/>
+      <c r="V51" s="101"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>2</v>
       </c>
-      <c r="B52" s="58"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="66"/>
-      <c r="G52" s="66"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="53"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="58"/>
-      <c r="M52" s="53"/>
-      <c r="N52" s="53"/>
-      <c r="O52" s="53"/>
-      <c r="P52" s="50"/>
-      <c r="Q52" s="51"/>
-      <c r="R52" s="51"/>
-      <c r="S52" s="51"/>
-      <c r="T52" s="52"/>
-      <c r="U52" s="53"/>
-      <c r="V52" s="59"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="83"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="134"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="135"/>
+      <c r="H52" s="115"/>
+      <c r="I52" s="84"/>
+      <c r="J52" s="83"/>
+      <c r="K52" s="84"/>
+      <c r="L52" s="115"/>
+      <c r="M52" s="83"/>
+      <c r="N52" s="83"/>
+      <c r="O52" s="83"/>
+      <c r="P52" s="80"/>
+      <c r="Q52" s="81"/>
+      <c r="R52" s="81"/>
+      <c r="S52" s="81"/>
+      <c r="T52" s="82"/>
+      <c r="U52" s="83"/>
+      <c r="V52" s="84"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>3</v>
       </c>
-      <c r="B53" s="58"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="65"/>
-      <c r="F53" s="66"/>
-      <c r="G53" s="66"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="59"/>
-      <c r="L53" s="58"/>
-      <c r="M53" s="53"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53"/>
-      <c r="P53" s="50"/>
-      <c r="Q53" s="51"/>
-      <c r="R53" s="51"/>
-      <c r="S53" s="51"/>
-      <c r="T53" s="52"/>
-      <c r="U53" s="53"/>
-      <c r="V53" s="59"/>
+      <c r="B53" s="115"/>
+      <c r="C53" s="83"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="134"/>
+      <c r="F53" s="135"/>
+      <c r="G53" s="135"/>
+      <c r="H53" s="115"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="83"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="115"/>
+      <c r="M53" s="83"/>
+      <c r="N53" s="83"/>
+      <c r="O53" s="83"/>
+      <c r="P53" s="80"/>
+      <c r="Q53" s="81"/>
+      <c r="R53" s="81"/>
+      <c r="S53" s="81"/>
+      <c r="T53" s="82"/>
+      <c r="U53" s="83"/>
+      <c r="V53" s="84"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>4</v>
       </c>
-      <c r="B54" s="58"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="65"/>
-      <c r="F54" s="66"/>
-      <c r="G54" s="66"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="59"/>
-      <c r="J54" s="53"/>
-      <c r="K54" s="59"/>
-      <c r="L54" s="58"/>
-      <c r="M54" s="53"/>
-      <c r="N54" s="53"/>
-      <c r="O54" s="53"/>
-      <c r="P54" s="50"/>
-      <c r="Q54" s="51"/>
-      <c r="R54" s="51"/>
-      <c r="S54" s="51"/>
-      <c r="T54" s="52"/>
-      <c r="U54" s="53"/>
-      <c r="V54" s="59"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="134"/>
+      <c r="F54" s="135"/>
+      <c r="G54" s="135"/>
+      <c r="H54" s="115"/>
+      <c r="I54" s="84"/>
+      <c r="J54" s="83"/>
+      <c r="K54" s="84"/>
+      <c r="L54" s="115"/>
+      <c r="M54" s="83"/>
+      <c r="N54" s="83"/>
+      <c r="O54" s="83"/>
+      <c r="P54" s="80"/>
+      <c r="Q54" s="81"/>
+      <c r="R54" s="81"/>
+      <c r="S54" s="81"/>
+      <c r="T54" s="82"/>
+      <c r="U54" s="83"/>
+      <c r="V54" s="84"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>5</v>
       </c>
-      <c r="B55" s="58"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="65"/>
-      <c r="F55" s="66"/>
-      <c r="G55" s="66"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="53"/>
-      <c r="K55" s="59"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="53"/>
-      <c r="N55" s="53"/>
-      <c r="O55" s="53"/>
-      <c r="P55" s="50"/>
-      <c r="Q55" s="51"/>
-      <c r="R55" s="51"/>
-      <c r="S55" s="51"/>
-      <c r="T55" s="52"/>
-      <c r="U55" s="53"/>
-      <c r="V55" s="59"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="134"/>
+      <c r="F55" s="135"/>
+      <c r="G55" s="135"/>
+      <c r="H55" s="115"/>
+      <c r="I55" s="84"/>
+      <c r="J55" s="83"/>
+      <c r="K55" s="84"/>
+      <c r="L55" s="115"/>
+      <c r="M55" s="83"/>
+      <c r="N55" s="83"/>
+      <c r="O55" s="83"/>
+      <c r="P55" s="80"/>
+      <c r="Q55" s="81"/>
+      <c r="R55" s="81"/>
+      <c r="S55" s="81"/>
+      <c r="T55" s="82"/>
+      <c r="U55" s="83"/>
+      <c r="V55" s="84"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>6</v>
       </c>
-      <c r="B56" s="58"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="59"/>
-      <c r="E56" s="65"/>
-      <c r="F56" s="66"/>
-      <c r="G56" s="66"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="59"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="59"/>
-      <c r="L56" s="58"/>
-      <c r="M56" s="53"/>
-      <c r="N56" s="53"/>
-      <c r="O56" s="53"/>
-      <c r="P56" s="50"/>
-      <c r="Q56" s="51"/>
-      <c r="R56" s="51"/>
-      <c r="S56" s="51"/>
-      <c r="T56" s="52"/>
-      <c r="U56" s="53"/>
-      <c r="V56" s="59"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="134"/>
+      <c r="F56" s="135"/>
+      <c r="G56" s="135"/>
+      <c r="H56" s="115"/>
+      <c r="I56" s="84"/>
+      <c r="J56" s="83"/>
+      <c r="K56" s="84"/>
+      <c r="L56" s="115"/>
+      <c r="M56" s="83"/>
+      <c r="N56" s="83"/>
+      <c r="O56" s="83"/>
+      <c r="P56" s="80"/>
+      <c r="Q56" s="81"/>
+      <c r="R56" s="81"/>
+      <c r="S56" s="81"/>
+      <c r="T56" s="82"/>
+      <c r="U56" s="83"/>
+      <c r="V56" s="84"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>7</v>
       </c>
-      <c r="B57" s="58"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="65"/>
-      <c r="F57" s="66"/>
-      <c r="G57" s="66"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="59"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="59"/>
-      <c r="L57" s="58"/>
-      <c r="M57" s="53"/>
-      <c r="N57" s="53"/>
-      <c r="O57" s="53"/>
-      <c r="P57" s="50"/>
-      <c r="Q57" s="51"/>
-      <c r="R57" s="51"/>
-      <c r="S57" s="51"/>
-      <c r="T57" s="52"/>
-      <c r="U57" s="53"/>
-      <c r="V57" s="59"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="134"/>
+      <c r="F57" s="135"/>
+      <c r="G57" s="135"/>
+      <c r="H57" s="115"/>
+      <c r="I57" s="84"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="84"/>
+      <c r="L57" s="115"/>
+      <c r="M57" s="83"/>
+      <c r="N57" s="83"/>
+      <c r="O57" s="83"/>
+      <c r="P57" s="80"/>
+      <c r="Q57" s="81"/>
+      <c r="R57" s="81"/>
+      <c r="S57" s="81"/>
+      <c r="T57" s="82"/>
+      <c r="U57" s="83"/>
+      <c r="V57" s="84"/>
     </row>
     <row r="58" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="31">
         <v>8</v>
       </c>
-      <c r="B58" s="60"/>
-      <c r="C58" s="54"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="67"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="68"/>
-      <c r="H58" s="60"/>
-      <c r="I58" s="61"/>
-      <c r="J58" s="54"/>
-      <c r="K58" s="61"/>
-      <c r="L58" s="60"/>
-      <c r="M58" s="54"/>
-      <c r="N58" s="54"/>
-      <c r="O58" s="54"/>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="57"/>
-      <c r="R58" s="57"/>
-      <c r="S58" s="57"/>
-      <c r="T58" s="55"/>
-      <c r="U58" s="54"/>
-      <c r="V58" s="61"/>
+      <c r="B58" s="114"/>
+      <c r="C58" s="88"/>
+      <c r="D58" s="89"/>
+      <c r="E58" s="136"/>
+      <c r="F58" s="137"/>
+      <c r="G58" s="137"/>
+      <c r="H58" s="114"/>
+      <c r="I58" s="89"/>
+      <c r="J58" s="88"/>
+      <c r="K58" s="89"/>
+      <c r="L58" s="114"/>
+      <c r="M58" s="88"/>
+      <c r="N58" s="88"/>
+      <c r="O58" s="88"/>
+      <c r="P58" s="85"/>
+      <c r="Q58" s="86"/>
+      <c r="R58" s="86"/>
+      <c r="S58" s="86"/>
+      <c r="T58" s="87"/>
+      <c r="U58" s="88"/>
+      <c r="V58" s="89"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="25"/>
-      <c r="B59" s="76"/>
-      <c r="C59" s="76"/>
-      <c r="V59" s="76"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="49"/>
+      <c r="V59" s="49"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B60" s="76" t="s">
+      <c r="B60" s="49" t="s">
         <v>19</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B61" s="76" t="s">
+      <c r="B61" s="49" t="s">
         <v>20</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B62" s="76"/>
+      <c r="B62" s="49"/>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B63" s="125" t="s">
+      <c r="B63" s="71" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B64" s="125" t="s">
-        <v>33</v>
-      </c>
-      <c r="E64" s="126"/>
-      <c r="F64" s="127"/>
-      <c r="G64" s="127"/>
-      <c r="H64" s="127"/>
-      <c r="I64" s="127"/>
-      <c r="J64" s="127"/>
-      <c r="K64" s="127"/>
-      <c r="L64" s="127"/>
-      <c r="M64" s="127"/>
-      <c r="N64" s="127"/>
-      <c r="O64" s="127"/>
-      <c r="P64" s="127"/>
-      <c r="Q64" s="127"/>
-      <c r="R64" s="127"/>
-      <c r="S64" s="127"/>
-      <c r="T64" s="127"/>
+      <c r="B64" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" s="72"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="73"/>
+      <c r="I64" s="73"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73"/>
+      <c r="L64" s="73"/>
+      <c r="M64" s="73"/>
+      <c r="N64" s="73"/>
+      <c r="O64" s="73"/>
+      <c r="P64" s="73"/>
+      <c r="Q64" s="73"/>
+      <c r="R64" s="73"/>
+      <c r="S64" s="73"/>
+      <c r="T64" s="73"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uWinYRKwa7C7VHKbsK2r/aKqpXn0Nq82JtlMGsuKgHu0rk8Iw3fAgcJpwopNet2JHgY9k7SjaJRJratuUtlnwQ==" saltValue="ltdgrW7T0OANh5QNwNyAnA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="74">
-    <mergeCell ref="P57:T57"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="P58:T58"/>
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="P50:T50"/>
-    <mergeCell ref="U50:V50"/>
-    <mergeCell ref="P51:T51"/>
-    <mergeCell ref="U51:V51"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L58:O58"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L56:O56"/>
-    <mergeCell ref="L57:O57"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="C7:R7"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="E55:G55"/>
     <mergeCell ref="B55:D55"/>
     <mergeCell ref="J51:K51"/>
     <mergeCell ref="J52:K52"/>
@@ -3308,22 +3297,38 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="E53:G53"/>
     <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="C7:R7"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:O50"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="L58:O58"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L56:O56"/>
+    <mergeCell ref="L57:O57"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="P50:T50"/>
+    <mergeCell ref="U50:V50"/>
+    <mergeCell ref="P51:T51"/>
+    <mergeCell ref="U51:V51"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="P57:T57"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="P58:T58"/>
+    <mergeCell ref="U58:V58"/>
+    <mergeCell ref="V9:V10"/>
     <mergeCell ref="P54:T54"/>
     <mergeCell ref="U54:V54"/>
     <mergeCell ref="P55:T55"/>
@@ -3336,7 +3341,7 @@
     <mergeCell ref="U53:V53"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations xWindow="527" yWindow="401" count="17">
+  <dataValidations xWindow="527" yWindow="401" count="13">
     <dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" errorTitle="Разряд" error="Выберите разряд спортсмена. В случае отсутствия разряда выберите &quot;б/р&quot;" promptTitle="Подсказка" prompt="Выберите разряд из списка. Для спортсменов/спортсменок без разряда выберите пункт &quot;б/р&quot;" sqref="F11:F48" xr:uid="{EA3CC518-E4BF-4BD9-9743-DF4855C8B284}">
       <formula1>"МСМК,МС,КМС,I,II,III,1юн.,2юн.,3юн.,б/р"</formula1>
     </dataValidation>
@@ -3361,35 +3366,23 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Выберите судейскую категорию из списка." sqref="M53:O57 L51:L58" xr:uid="{BC1FB9AE-024A-481D-8DEA-68641A86D77B}">
       <formula1>"Всероссийская,Первая,Вторая,Третья,б/к"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ошибка" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="G23:G48" xr:uid="{34405025-C693-4ADB-9A18-67164ECD3983}">
-      <formula1>AND(YEAR(TODAY())&lt;YEAR(E23)+13,G23="+")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="J23:J48" xr:uid="{D72ED731-57A8-4341-9EB1-695717413BC2}">
-      <formula1>AND(YEAR(TODAY())&gt;YEAR(E23)+14,J23="+")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="H23:H48" xr:uid="{AABE62F5-3A3E-4059-A10C-F41F09122F12}">
-      <formula1>AND(YEAR(TODAY())&gt;YEAR(E23)+12,YEAR(TODAY())&lt;YEAR(E23)+16,H23="+")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="I23:I48" xr:uid="{FAF1706F-B09D-42E8-839B-5945854EE43C}">
-      <formula1>AND(YEAR(TODAY())&gt;YEAR(E23)+14,YEAR(TODAY())&lt;YEAR(E23)+19,I23="+")</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Отметка должна состоять из неповторяющегося номера группы и букв К или Р (для резерва)." sqref="P23:P48" xr:uid="{1C158208-20D0-4CCA-95EB-E44BDC9B91F4}">
       <formula1>AND(ISNUMBER(_xlfn.NUMBERVALUE(LEFT(P23,1))),OR(RIGHT(P23,1)="К",RIGHT(P23,1)="Р"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="J11:J22" xr:uid="{1BC43E25-B0E9-475F-A6EA-C0ED1D30E998}">
-      <formula1>AND(YEAR(TODAY())&gt;$C11+14,J11="+")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="H11:H48" xr:uid="{863475AF-F157-4781-8457-0CAB3400DB87}">
+      <formula1>AND(YEAR(TODAY())&gt;YEAR($E11)+12,YEAR(TODAY())&lt;YEAR($E11)+16,H11="+")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="I11:I22" xr:uid="{C77490BC-C873-4861-84C3-F8E66ECD3D78}">
-      <formula1>AND(YEAR(TODAY())&gt;$C11+14,YEAR(TODAY())&lt;$C11+19,I11="+")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ошибка" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="G11:G48" xr:uid="{C255EDE3-F357-42B9-9445-0C586E43AC09}">
+      <formula1>AND(YEAR(TODAY())&lt;YEAR($E11)+13,G11="+")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="H11:H22" xr:uid="{A7A5E8BA-9936-46FB-9C4B-A16B3E1D5BF9}">
-      <formula1>AND(YEAR(TODAY())&gt;$C11+12,YEAR(TODAY())&lt;$C11+16,H11="+")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="I11:I48" xr:uid="{BAB1D315-6F86-48F1-B5C9-CC9BABFB307F}">
+      <formula1>AND(YEAR(TODAY())&gt;YEAR($E11)+14,YEAR(TODAY())&lt;YEAR($E11)+19,I11="+")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ошибка" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="G11:G22" xr:uid="{01BBC3B9-F6D0-45EC-9612-576FED877118}">
-      <formula1>AND(YEAR(TODAY())&lt;E11+13,G11="+")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="J11:J48" xr:uid="{80282FCE-E3E1-4930-AF07-D7EF299E39CD}">
+      <formula1>AND(YEAR(TODAY())&gt;YEAR($E11)+14,J11="+")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change age rules for one competition;
</commit_message>
<xml_diff>
--- a/assets/Заявка.xlsx
+++ b/assets/Заявка.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Игорь\WebstormProjects\synchroreg\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF7FF91-257F-4DDA-AA92-90ACFC39BB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF9DFA1-B820-465F-9F25-73A73851357B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>ТЕХНИЧЕСКАЯ ЗАЯВКА</t>
   </si>
@@ -69,9 +69,6 @@
     <t>&lt;13</t>
   </si>
   <si>
-    <t>13-15</t>
-  </si>
-  <si>
     <t>15-18</t>
   </si>
   <si>
@@ -150,10 +147,10 @@
     <t>Приказ о продлении категории</t>
   </si>
   <si>
-    <t>qe</t>
-  </si>
-  <si>
     <t>&gt;15</t>
+  </si>
+  <si>
+    <t>12-15</t>
   </si>
 </sst>
 </file>
@@ -940,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1213,15 +1210,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1233,15 +1222,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1253,36 +1234,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1294,55 +1246,29 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1384,33 +1310,107 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1796,19 +1796,19 @@
     </row>
     <row r="3" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="47"/>
     </row>
     <row r="5" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="47"/>
     </row>
@@ -1816,135 +1816,133 @@
       <c r="B7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="118"/>
-      <c r="M7" s="118"/>
-      <c r="N7" s="118"/>
-      <c r="O7" s="118"/>
-      <c r="P7" s="118"/>
-      <c r="Q7" s="118"/>
-      <c r="R7" s="118"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="95"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="95"/>
     </row>
     <row r="8" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102" t="s">
+      <c r="A9" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="110" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="111"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="115" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="117" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="102" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="103"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="103"/>
+      <c r="O9" s="103"/>
+      <c r="P9" s="104"/>
+      <c r="Q9" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
+      <c r="T9" s="107"/>
+      <c r="U9" s="128" t="s">
+        <v>20</v>
+      </c>
+      <c r="V9" s="136" t="s">
+        <v>30</v>
+      </c>
+      <c r="W9" s="120" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="26" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="109"/>
+      <c r="B10" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="107" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="109" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="111" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="112"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="125" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="126"/>
-      <c r="M9" s="126"/>
-      <c r="N9" s="126"/>
-      <c r="O9" s="126"/>
-      <c r="P9" s="127"/>
-      <c r="Q9" s="128" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" s="129"/>
-      <c r="S9" s="129"/>
-      <c r="T9" s="130"/>
-      <c r="U9" s="116" t="s">
-        <v>21</v>
-      </c>
-      <c r="V9" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="W9" s="92" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" s="26" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="103"/>
-      <c r="B10" s="51" t="s">
+      <c r="C10" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="D10" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="108"/>
-      <c r="F10" s="110"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="116"/>
       <c r="G10" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="55" t="s">
+      <c r="H10" s="138" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="55" t="s">
-        <v>12</v>
-      </c>
       <c r="J10" s="56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K10" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="58" t="s">
+      <c r="M10" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="58" t="s">
+      <c r="N10" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="58" t="s">
+      <c r="O10" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="58" t="s">
+      <c r="P10" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="59" t="s">
-        <v>27</v>
-      </c>
       <c r="Q10" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="61" t="s">
+      <c r="S10" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="61" t="s">
+      <c r="T10" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="T10" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="U10" s="117"/>
-      <c r="V10" s="91"/>
-      <c r="W10" s="93"/>
+      <c r="U10" s="129"/>
+      <c r="V10" s="137"/>
+      <c r="W10" s="121"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="46"/>
       <c r="D11" s="63"/>
       <c r="E11" s="66"/>
@@ -2971,249 +2969,249 @@
     </row>
     <row r="50" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="32"/>
-      <c r="B50" s="121" t="s">
+      <c r="B50" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="122"/>
-      <c r="D50" s="123"/>
-      <c r="E50" s="119" t="s">
+      <c r="C50" s="99"/>
+      <c r="D50" s="100"/>
+      <c r="E50" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="124"/>
-      <c r="G50" s="124"/>
-      <c r="H50" s="119" t="s">
+      <c r="F50" s="101"/>
+      <c r="G50" s="101"/>
+      <c r="H50" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="I50" s="120"/>
-      <c r="J50" s="124" t="s">
+      <c r="I50" s="97"/>
+      <c r="J50" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="K50" s="124"/>
-      <c r="L50" s="119" t="s">
+      <c r="K50" s="101"/>
+      <c r="L50" s="96" t="s">
+        <v>27</v>
+      </c>
+      <c r="M50" s="101"/>
+      <c r="N50" s="101"/>
+      <c r="O50" s="101"/>
+      <c r="P50" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="M50" s="124"/>
-      <c r="N50" s="124"/>
-      <c r="O50" s="124"/>
-      <c r="P50" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q50" s="95"/>
-      <c r="R50" s="95"/>
-      <c r="S50" s="95"/>
-      <c r="T50" s="96"/>
-      <c r="U50" s="94" t="s">
-        <v>37</v>
-      </c>
-      <c r="V50" s="95"/>
+      <c r="Q50" s="123"/>
+      <c r="R50" s="123"/>
+      <c r="S50" s="123"/>
+      <c r="T50" s="124"/>
+      <c r="U50" s="122" t="s">
+        <v>36</v>
+      </c>
+      <c r="V50" s="123"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="29">
         <v>1</v>
       </c>
-      <c r="B51" s="131"/>
-      <c r="C51" s="100"/>
-      <c r="D51" s="101"/>
-      <c r="E51" s="132"/>
-      <c r="F51" s="133"/>
-      <c r="G51" s="133"/>
-      <c r="H51" s="131"/>
-      <c r="I51" s="101"/>
-      <c r="J51" s="100"/>
-      <c r="K51" s="101"/>
-      <c r="L51" s="131"/>
-      <c r="M51" s="100"/>
-      <c r="N51" s="100"/>
-      <c r="O51" s="100"/>
-      <c r="P51" s="97"/>
-      <c r="Q51" s="98"/>
-      <c r="R51" s="98"/>
-      <c r="S51" s="98"/>
-      <c r="T51" s="99"/>
-      <c r="U51" s="100"/>
-      <c r="V51" s="101"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="88"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="94"/>
+      <c r="G51" s="94"/>
+      <c r="H51" s="86"/>
+      <c r="I51" s="88"/>
+      <c r="J51" s="87"/>
+      <c r="K51" s="88"/>
+      <c r="L51" s="86"/>
+      <c r="M51" s="87"/>
+      <c r="N51" s="87"/>
+      <c r="O51" s="87"/>
+      <c r="P51" s="125"/>
+      <c r="Q51" s="126"/>
+      <c r="R51" s="126"/>
+      <c r="S51" s="126"/>
+      <c r="T51" s="127"/>
+      <c r="U51" s="87"/>
+      <c r="V51" s="88"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>2</v>
       </c>
-      <c r="B52" s="115"/>
-      <c r="C52" s="83"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="134"/>
-      <c r="F52" s="135"/>
-      <c r="G52" s="135"/>
-      <c r="H52" s="115"/>
-      <c r="I52" s="84"/>
-      <c r="J52" s="83"/>
-      <c r="K52" s="84"/>
-      <c r="L52" s="115"/>
-      <c r="M52" s="83"/>
-      <c r="N52" s="83"/>
-      <c r="O52" s="83"/>
-      <c r="P52" s="80"/>
-      <c r="Q52" s="81"/>
-      <c r="R52" s="81"/>
-      <c r="S52" s="81"/>
-      <c r="T52" s="82"/>
-      <c r="U52" s="83"/>
-      <c r="V52" s="84"/>
+      <c r="B52" s="80"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="82"/>
+      <c r="J52" s="81"/>
+      <c r="K52" s="82"/>
+      <c r="L52" s="80"/>
+      <c r="M52" s="81"/>
+      <c r="N52" s="81"/>
+      <c r="O52" s="81"/>
+      <c r="P52" s="130"/>
+      <c r="Q52" s="131"/>
+      <c r="R52" s="131"/>
+      <c r="S52" s="131"/>
+      <c r="T52" s="132"/>
+      <c r="U52" s="81"/>
+      <c r="V52" s="82"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>3</v>
       </c>
-      <c r="B53" s="115"/>
-      <c r="C53" s="83"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="134"/>
-      <c r="F53" s="135"/>
-      <c r="G53" s="135"/>
-      <c r="H53" s="115"/>
-      <c r="I53" s="84"/>
-      <c r="J53" s="83"/>
-      <c r="K53" s="84"/>
-      <c r="L53" s="115"/>
-      <c r="M53" s="83"/>
-      <c r="N53" s="83"/>
-      <c r="O53" s="83"/>
-      <c r="P53" s="80"/>
-      <c r="Q53" s="81"/>
-      <c r="R53" s="81"/>
-      <c r="S53" s="81"/>
-      <c r="T53" s="82"/>
-      <c r="U53" s="83"/>
-      <c r="V53" s="84"/>
+      <c r="B53" s="80"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="90"/>
+      <c r="G53" s="90"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="82"/>
+      <c r="J53" s="81"/>
+      <c r="K53" s="82"/>
+      <c r="L53" s="80"/>
+      <c r="M53" s="81"/>
+      <c r="N53" s="81"/>
+      <c r="O53" s="81"/>
+      <c r="P53" s="130"/>
+      <c r="Q53" s="131"/>
+      <c r="R53" s="131"/>
+      <c r="S53" s="131"/>
+      <c r="T53" s="132"/>
+      <c r="U53" s="81"/>
+      <c r="V53" s="82"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>4</v>
       </c>
-      <c r="B54" s="115"/>
-      <c r="C54" s="83"/>
-      <c r="D54" s="84"/>
-      <c r="E54" s="134"/>
-      <c r="F54" s="135"/>
-      <c r="G54" s="135"/>
-      <c r="H54" s="115"/>
-      <c r="I54" s="84"/>
-      <c r="J54" s="83"/>
-      <c r="K54" s="84"/>
-      <c r="L54" s="115"/>
-      <c r="M54" s="83"/>
-      <c r="N54" s="83"/>
-      <c r="O54" s="83"/>
-      <c r="P54" s="80"/>
-      <c r="Q54" s="81"/>
-      <c r="R54" s="81"/>
-      <c r="S54" s="81"/>
-      <c r="T54" s="82"/>
-      <c r="U54" s="83"/>
-      <c r="V54" s="84"/>
+      <c r="B54" s="80"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="82"/>
+      <c r="E54" s="89"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="90"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="82"/>
+      <c r="J54" s="81"/>
+      <c r="K54" s="82"/>
+      <c r="L54" s="80"/>
+      <c r="M54" s="81"/>
+      <c r="N54" s="81"/>
+      <c r="O54" s="81"/>
+      <c r="P54" s="130"/>
+      <c r="Q54" s="131"/>
+      <c r="R54" s="131"/>
+      <c r="S54" s="131"/>
+      <c r="T54" s="132"/>
+      <c r="U54" s="81"/>
+      <c r="V54" s="82"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>5</v>
       </c>
-      <c r="B55" s="115"/>
-      <c r="C55" s="83"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="134"/>
-      <c r="F55" s="135"/>
-      <c r="G55" s="135"/>
-      <c r="H55" s="115"/>
-      <c r="I55" s="84"/>
-      <c r="J55" s="83"/>
-      <c r="K55" s="84"/>
-      <c r="L55" s="115"/>
-      <c r="M55" s="83"/>
-      <c r="N55" s="83"/>
-      <c r="O55" s="83"/>
-      <c r="P55" s="80"/>
-      <c r="Q55" s="81"/>
-      <c r="R55" s="81"/>
-      <c r="S55" s="81"/>
-      <c r="T55" s="82"/>
-      <c r="U55" s="83"/>
-      <c r="V55" s="84"/>
+      <c r="B55" s="80"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="82"/>
+      <c r="E55" s="89"/>
+      <c r="F55" s="90"/>
+      <c r="G55" s="90"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="82"/>
+      <c r="J55" s="81"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="80"/>
+      <c r="M55" s="81"/>
+      <c r="N55" s="81"/>
+      <c r="O55" s="81"/>
+      <c r="P55" s="130"/>
+      <c r="Q55" s="131"/>
+      <c r="R55" s="131"/>
+      <c r="S55" s="131"/>
+      <c r="T55" s="132"/>
+      <c r="U55" s="81"/>
+      <c r="V55" s="82"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>6</v>
       </c>
-      <c r="B56" s="115"/>
-      <c r="C56" s="83"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="134"/>
-      <c r="F56" s="135"/>
-      <c r="G56" s="135"/>
-      <c r="H56" s="115"/>
-      <c r="I56" s="84"/>
-      <c r="J56" s="83"/>
-      <c r="K56" s="84"/>
-      <c r="L56" s="115"/>
-      <c r="M56" s="83"/>
-      <c r="N56" s="83"/>
-      <c r="O56" s="83"/>
-      <c r="P56" s="80"/>
-      <c r="Q56" s="81"/>
-      <c r="R56" s="81"/>
-      <c r="S56" s="81"/>
-      <c r="T56" s="82"/>
-      <c r="U56" s="83"/>
-      <c r="V56" s="84"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="81"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="89"/>
+      <c r="F56" s="90"/>
+      <c r="G56" s="90"/>
+      <c r="H56" s="80"/>
+      <c r="I56" s="82"/>
+      <c r="J56" s="81"/>
+      <c r="K56" s="82"/>
+      <c r="L56" s="80"/>
+      <c r="M56" s="81"/>
+      <c r="N56" s="81"/>
+      <c r="O56" s="81"/>
+      <c r="P56" s="130"/>
+      <c r="Q56" s="131"/>
+      <c r="R56" s="131"/>
+      <c r="S56" s="131"/>
+      <c r="T56" s="132"/>
+      <c r="U56" s="81"/>
+      <c r="V56" s="82"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>7</v>
       </c>
-      <c r="B57" s="115"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="134"/>
-      <c r="F57" s="135"/>
-      <c r="G57" s="135"/>
-      <c r="H57" s="115"/>
-      <c r="I57" s="84"/>
-      <c r="J57" s="83"/>
-      <c r="K57" s="84"/>
-      <c r="L57" s="115"/>
-      <c r="M57" s="83"/>
-      <c r="N57" s="83"/>
-      <c r="O57" s="83"/>
-      <c r="P57" s="80"/>
-      <c r="Q57" s="81"/>
-      <c r="R57" s="81"/>
-      <c r="S57" s="81"/>
-      <c r="T57" s="82"/>
-      <c r="U57" s="83"/>
-      <c r="V57" s="84"/>
+      <c r="B57" s="80"/>
+      <c r="C57" s="81"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="90"/>
+      <c r="G57" s="90"/>
+      <c r="H57" s="80"/>
+      <c r="I57" s="82"/>
+      <c r="J57" s="81"/>
+      <c r="K57" s="82"/>
+      <c r="L57" s="80"/>
+      <c r="M57" s="81"/>
+      <c r="N57" s="81"/>
+      <c r="O57" s="81"/>
+      <c r="P57" s="130"/>
+      <c r="Q57" s="131"/>
+      <c r="R57" s="131"/>
+      <c r="S57" s="131"/>
+      <c r="T57" s="132"/>
+      <c r="U57" s="81"/>
+      <c r="V57" s="82"/>
     </row>
     <row r="58" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="31">
         <v>8</v>
       </c>
-      <c r="B58" s="114"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="89"/>
-      <c r="E58" s="136"/>
-      <c r="F58" s="137"/>
-      <c r="G58" s="137"/>
-      <c r="H58" s="114"/>
-      <c r="I58" s="89"/>
-      <c r="J58" s="88"/>
-      <c r="K58" s="89"/>
-      <c r="L58" s="114"/>
-      <c r="M58" s="88"/>
-      <c r="N58" s="88"/>
-      <c r="O58" s="88"/>
-      <c r="P58" s="85"/>
-      <c r="Q58" s="86"/>
-      <c r="R58" s="86"/>
-      <c r="S58" s="86"/>
-      <c r="T58" s="87"/>
-      <c r="U58" s="88"/>
-      <c r="V58" s="89"/>
+      <c r="B58" s="83"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="91"/>
+      <c r="F58" s="92"/>
+      <c r="G58" s="92"/>
+      <c r="H58" s="83"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="84"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="83"/>
+      <c r="M58" s="84"/>
+      <c r="N58" s="84"/>
+      <c r="O58" s="84"/>
+      <c r="P58" s="133"/>
+      <c r="Q58" s="134"/>
+      <c r="R58" s="134"/>
+      <c r="S58" s="134"/>
+      <c r="T58" s="135"/>
+      <c r="U58" s="84"/>
+      <c r="V58" s="85"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="25"/>
@@ -3223,13 +3221,13 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B60" s="49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B61" s="49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -3243,7 +3241,7 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B64" s="71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E64" s="72"/>
       <c r="F64" s="73"/>
@@ -3265,6 +3263,64 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="74">
+    <mergeCell ref="P57:T57"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="P58:T58"/>
+    <mergeCell ref="U58:V58"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="P54:T54"/>
+    <mergeCell ref="U54:V54"/>
+    <mergeCell ref="P55:T55"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="P56:T56"/>
+    <mergeCell ref="U56:V56"/>
+    <mergeCell ref="P52:T52"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="P53:T53"/>
+    <mergeCell ref="U53:V53"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="P50:T50"/>
+    <mergeCell ref="U50:V50"/>
+    <mergeCell ref="P51:T51"/>
+    <mergeCell ref="U51:V51"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L58:O58"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L56:O56"/>
+    <mergeCell ref="L57:O57"/>
+    <mergeCell ref="C7:R7"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:O50"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="L52:O52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="L55:O55"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
@@ -3281,67 +3337,9 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="E55:G55"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="L51:O51"/>
-    <mergeCell ref="L52:O52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="L55:O55"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="C7:R7"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="L50:O50"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="Q9:T9"/>
-    <mergeCell ref="L58:O58"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="L56:O56"/>
-    <mergeCell ref="L57:O57"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="P50:T50"/>
-    <mergeCell ref="U50:V50"/>
-    <mergeCell ref="P51:T51"/>
-    <mergeCell ref="U51:V51"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="P57:T57"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="P58:T58"/>
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="P54:T54"/>
-    <mergeCell ref="U54:V54"/>
-    <mergeCell ref="P55:T55"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="P56:T56"/>
-    <mergeCell ref="U56:V56"/>
-    <mergeCell ref="P52:T52"/>
-    <mergeCell ref="U52:V52"/>
-    <mergeCell ref="P53:T53"/>
-    <mergeCell ref="U53:V53"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations xWindow="527" yWindow="401" count="13">
+  <dataValidations xWindow="527" yWindow="401" count="14">
     <dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" errorTitle="Разряд" error="Выберите разряд спортсмена. В случае отсутствия разряда выберите &quot;б/р&quot;" promptTitle="Подсказка" prompt="Выберите разряд из списка. Для спортсменов/спортсменок без разряда выберите пункт &quot;б/р&quot;" sqref="F11:F48" xr:uid="{EA3CC518-E4BF-4BD9-9743-DF4855C8B284}">
       <formula1>"МСМК,МС,КМС,I,II,III,1юн.,2юн.,3юн.,б/р"</formula1>
     </dataValidation>
@@ -3369,11 +3367,8 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Подсказка" prompt="Отметка должна состоять из неповторяющегося номера группы и букв К или Р (для резерва)." sqref="P23:P48" xr:uid="{1C158208-20D0-4CCA-95EB-E44BDC9B91F4}">
       <formula1>AND(ISNUMBER(_xlfn.NUMBERVALUE(LEFT(P23,1))),OR(RIGHT(P23,1)="К",RIGHT(P23,1)="Р"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="H11:H48" xr:uid="{863475AF-F157-4781-8457-0CAB3400DB87}">
-      <formula1>AND(YEAR(TODAY())&gt;YEAR($E11)+12,YEAR(TODAY())&lt;YEAR($E11)+16,H11="+")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ошибка" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="G11:G48" xr:uid="{C255EDE3-F357-42B9-9445-0C586E43AC09}">
-      <formula1>AND(YEAR(TODAY())&lt;YEAR($E11)+13,G11="+")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ошибка" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="G12:G48" xr:uid="{C255EDE3-F357-42B9-9445-0C586E43AC09}">
+      <formula1>AND(YEAR(TODAY())&lt;YEAR($E12)+13,G12="+")</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="I11:I48" xr:uid="{BAB1D315-6F86-48F1-B5C9-CC9BABFB307F}">
       <formula1>AND(YEAR(TODAY())&gt;YEAR($E11)+14,YEAR(TODAY())&lt;YEAR($E11)+19,I11="+")</formula1>
@@ -3381,6 +3376,12 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="J11:J48" xr:uid="{80282FCE-E3E1-4930-AF07-D7EF299E39CD}">
       <formula1>AND(YEAR(TODAY())&gt;YEAR($E11)+14,J11="+")</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ошибка" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="G11" xr:uid="{3BEEDF42-9927-41F8-91FD-2E058BCB2522}">
+      <formula1>AND(YEAR(TODAY())&lt;YEAR($E11)+13,G11="+")</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Спортсмен не подходит по возрасту или отметкой не является символ &quot;+&quot;." promptTitle="Подсказка" prompt="Отметкой об участии должен быть исключительно символ &quot;+&quot;." sqref="H11:H45 H47:H48 H46" xr:uid="{19692730-760B-4C15-9EED-8F3E119370E6}">
+      <formula1>AND(YEAR(TODAY())&gt;YEAR($E11)+11,YEAR(TODAY())&lt;YEAR($E11)+16,H11="+")</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>

</xml_diff>